<commit_message>
Adding the initial fixed angle stand
Adding the print and design files for the initial fixed angle stand, and adding them into the BoM, the Maker Guide, and the User Guide
</commit_message>
<xml_diff>
--- a/Documentation/Working_Documents/LipSync_BOM.xlsx
+++ b/Documentation/Working_Documents/LipSync_BOM.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27126"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27231"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://neilsquiresoc.sharepoint.com/sites/MMC-RD/Shared Documents/RD 21-05 LipSync 4/LipSync4/Documentation/Working_Documents/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\bradw\GitHub\LipSync\Documentation\Working_Documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1782" documentId="11_DC0E2523FAFE28515E8D5C5A1D4A6B02C3B15AFA" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{428D312F-2597-4CCD-9180-BCD762F1C469}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{73E8C4BD-798C-4AFF-A214-1817A39EDCBA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="BOM - v4.0" sheetId="5" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="619" uniqueCount="363">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="625" uniqueCount="367">
   <si>
     <t>Total filament (g)</t>
   </si>
@@ -1125,6 +1125,18 @@
   </si>
   <si>
     <t>4.0</t>
+  </si>
+  <si>
+    <t>LS4_Hub_Stand_Front</t>
+  </si>
+  <si>
+    <t>LS4_Hub_Stand_Leg</t>
+  </si>
+  <si>
+    <t>Front of the default Hub stand</t>
+  </si>
+  <si>
+    <t>Leg for the default Hub stand</t>
   </si>
 </sst>
 </file>
@@ -1532,6 +1544,7 @@
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
     <xf numFmtId="0" fontId="7" fillId="5" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1541,7 +1554,6 @@
     <xf numFmtId="0" fontId="3" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
   </cellXfs>
   <cellStyles count="8">
     <cellStyle name="60% - Accent4" xfId="3" builtinId="44"/>
@@ -1831,38 +1843,38 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BDFDD599-C177-4BBC-A644-7A0346B01187}">
-  <dimension ref="A1:AG145"/>
+  <dimension ref="A1:AG147"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="1" ySplit="4" topLeftCell="B31" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="4" topLeftCell="B54" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A5" sqref="A5"/>
-      <selection pane="bottomRight" activeCell="C3" sqref="C3"/>
+      <selection pane="bottomRight" activeCell="E71" sqref="E71"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="14.140625" customWidth="1"/>
-    <col min="2" max="2" width="32.28515625" customWidth="1"/>
-    <col min="3" max="3" width="45.42578125" customWidth="1"/>
-    <col min="4" max="4" width="21.7109375" customWidth="1"/>
-    <col min="5" max="5" width="19.140625" customWidth="1"/>
-    <col min="6" max="6" width="8.42578125" customWidth="1"/>
-    <col min="7" max="7" width="21.140625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="6.140625" customWidth="1"/>
-    <col min="9" max="9" width="9.140625" customWidth="1"/>
-    <col min="10" max="10" width="5.42578125" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="16.140625" customWidth="1"/>
-    <col min="12" max="12" width="15.140625" customWidth="1"/>
-    <col min="13" max="13" width="10.28515625" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="7.5703125" customWidth="1"/>
-    <col min="15" max="15" width="78.7109375" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="17.7109375" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="12.28515625" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="89.85546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="14.109375" customWidth="1"/>
+    <col min="2" max="2" width="32.33203125" customWidth="1"/>
+    <col min="3" max="3" width="45.44140625" customWidth="1"/>
+    <col min="4" max="4" width="21.6640625" customWidth="1"/>
+    <col min="5" max="5" width="19.109375" customWidth="1"/>
+    <col min="6" max="6" width="8.44140625" customWidth="1"/>
+    <col min="7" max="7" width="21.109375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="6.109375" customWidth="1"/>
+    <col min="9" max="9" width="9.109375" customWidth="1"/>
+    <col min="10" max="10" width="5.44140625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="16.109375" customWidth="1"/>
+    <col min="12" max="12" width="15.109375" customWidth="1"/>
+    <col min="13" max="13" width="10.33203125" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="7.5546875" customWidth="1"/>
+    <col min="15" max="15" width="78.6640625" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="17.6640625" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="12.33203125" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="89.88671875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" ht="35.25" x14ac:dyDescent="0.5">
+    <row r="1" spans="1:17" ht="36" x14ac:dyDescent="0.65">
       <c r="B1" s="1" t="s">
         <v>308</v>
       </c>
@@ -1879,11 +1891,11 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:17" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:17" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B2" s="13" t="s">
         <v>4</v>
       </c>
-      <c r="C2" s="58" t="s">
+      <c r="C2" s="55" t="s">
         <v>362</v>
       </c>
       <c r="E2" t="s">
@@ -1894,28 +1906,28 @@
       </c>
       <c r="G2" s="11"/>
       <c r="I2" s="6">
-        <f>SUM(I54:I70)</f>
-        <v>158</v>
+        <f>SUM(I54:I72)</f>
+        <v>175</v>
       </c>
       <c r="L2" s="22">
-        <f>SUM(L6:L45,L48:L50,L54:L70)</f>
-        <v>176.62886666666662</v>
+        <f>SUM(L6:L45,L48:L50,L54:L72)</f>
+        <v>177.13886666666662</v>
       </c>
       <c r="M2" s="5">
-        <f>SUM(M6:M70)</f>
-        <v>325.8399999999998</v>
+        <f>SUM(M6:M72)</f>
+        <v>326.3499999999998</v>
       </c>
       <c r="N2" s="23">
-        <f>SUM(N54:N70)</f>
-        <v>0.62708333333333344</v>
-      </c>
-    </row>
-    <row r="3" spans="1:17" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+        <f>SUM(N54:N72)</f>
+        <v>0.64652777777777781</v>
+      </c>
+    </row>
+    <row r="3" spans="1:17" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B3" s="14" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="4" spans="1:17" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:17" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A4" s="14" t="s">
         <v>7</v>
       </c>
@@ -1962,12 +1974,12 @@
       </c>
       <c r="Q4" s="7"/>
     </row>
-    <row r="5" spans="1:17" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A5" s="55" t="s">
+    <row r="5" spans="1:17" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A5" s="56" t="s">
         <v>306</v>
       </c>
-      <c r="B5" s="55"/>
-      <c r="C5" s="55"/>
+      <c r="B5" s="56"/>
+      <c r="C5" s="56"/>
       <c r="D5" s="45"/>
       <c r="E5" s="45"/>
       <c r="F5" s="45"/>
@@ -1983,7 +1995,7 @@
       <c r="P5" s="45"/>
       <c r="Q5" s="45"/>
     </row>
-    <row r="6" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>20</v>
       </c>
@@ -2030,7 +2042,7 @@
         <v>244</v>
       </c>
     </row>
-    <row r="7" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>26</v>
       </c>
@@ -2077,7 +2089,7 @@
         <v>245</v>
       </c>
     </row>
-    <row r="8" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>29</v>
       </c>
@@ -2124,7 +2136,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="9" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>33</v>
       </c>
@@ -2171,7 +2183,7 @@
         <v>247</v>
       </c>
     </row>
-    <row r="10" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>38</v>
       </c>
@@ -2218,7 +2230,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="11" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>319</v>
       </c>
@@ -2265,7 +2277,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="12" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>49</v>
       </c>
@@ -2312,7 +2324,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="13" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>59</v>
       </c>
@@ -2359,7 +2371,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="14" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>63</v>
       </c>
@@ -2406,7 +2418,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="15" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>74</v>
       </c>
@@ -2453,7 +2465,7 @@
         <v>253</v>
       </c>
     </row>
-    <row r="16" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>68</v>
       </c>
@@ -2500,7 +2512,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="17" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>109</v>
       </c>
@@ -2544,7 +2556,7 @@
         <v>151</v>
       </c>
     </row>
-    <row r="18" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
         <v>109</v>
       </c>
@@ -2586,12 +2598,12 @@
         <v>153</v>
       </c>
     </row>
-    <row r="19" spans="1:15" s="47" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A19" s="56" t="s">
+    <row r="19" spans="1:15" s="47" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A19" s="57" t="s">
         <v>303</v>
       </c>
-      <c r="B19" s="56"/>
-      <c r="C19" s="56"/>
+      <c r="B19" s="57"/>
+      <c r="C19" s="57"/>
       <c r="D19" s="46"/>
       <c r="G19" s="46"/>
       <c r="K19" s="48"/>
@@ -2599,7 +2611,7 @@
       <c r="M19" s="49"/>
       <c r="O19" s="50"/>
     </row>
-    <row r="20" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>55</v>
       </c>
@@ -2646,7 +2658,7 @@
         <v>252</v>
       </c>
     </row>
-    <row r="21" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>80</v>
       </c>
@@ -2693,7 +2705,7 @@
         <v>256</v>
       </c>
     </row>
-    <row r="22" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>85</v>
       </c>
@@ -2740,7 +2752,7 @@
         <v>255</v>
       </c>
     </row>
-    <row r="23" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
         <v>88</v>
       </c>
@@ -2787,7 +2799,7 @@
         <v>259</v>
       </c>
     </row>
-    <row r="24" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
         <v>93</v>
       </c>
@@ -2834,7 +2846,7 @@
         <v>260</v>
       </c>
     </row>
-    <row r="25" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
         <v>98</v>
       </c>
@@ -2881,7 +2893,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="26" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
         <v>104</v>
       </c>
@@ -2928,7 +2940,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="27" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
         <v>110</v>
       </c>
@@ -2975,7 +2987,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="28" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
         <v>114</v>
       </c>
@@ -3022,7 +3034,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="29" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
         <v>120</v>
       </c>
@@ -3069,7 +3081,7 @@
         <v>263</v>
       </c>
     </row>
-    <row r="30" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
         <v>125</v>
       </c>
@@ -3116,7 +3128,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="31" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
         <v>131</v>
       </c>
@@ -3163,7 +3175,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="32" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
         <v>136</v>
       </c>
@@ -3210,7 +3222,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="33" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
         <v>142</v>
       </c>
@@ -3257,7 +3269,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="34" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
         <v>158</v>
       </c>
@@ -3304,7 +3316,7 @@
         <v>163</v>
       </c>
     </row>
-    <row r="35" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
         <v>164</v>
       </c>
@@ -3351,7 +3363,7 @@
         <v>166</v>
       </c>
     </row>
-    <row r="36" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
         <v>178</v>
       </c>
@@ -3398,7 +3410,7 @@
         <v>266</v>
       </c>
     </row>
-    <row r="37" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
         <v>167</v>
       </c>
@@ -3445,7 +3457,7 @@
         <v>173</v>
       </c>
     </row>
-    <row r="38" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
         <v>109</v>
       </c>
@@ -3492,7 +3504,7 @@
         <v>265</v>
       </c>
     </row>
-    <row r="39" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
         <v>154</v>
       </c>
@@ -3536,14 +3548,14 @@
         <v>268</v>
       </c>
     </row>
-    <row r="40" spans="1:18" s="47" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A40" s="57" t="s">
+    <row r="40" spans="1:18" s="47" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A40" s="58" t="s">
         <v>304</v>
       </c>
-      <c r="B40" s="57"/>
-      <c r="C40" s="57"/>
-    </row>
-    <row r="41" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="B40" s="58"/>
+      <c r="C40" s="58"/>
+    </row>
+    <row r="41" spans="1:18" x14ac:dyDescent="0.3">
       <c r="B41" t="s">
         <v>299</v>
       </c>
@@ -3587,7 +3599,7 @@
         <v>301</v>
       </c>
     </row>
-    <row r="42" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:18" x14ac:dyDescent="0.3">
       <c r="B42" t="s">
         <v>295</v>
       </c>
@@ -3628,7 +3640,7 @@
         <v>294</v>
       </c>
     </row>
-    <row r="43" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A43" t="s">
         <v>109</v>
       </c>
@@ -3672,7 +3684,7 @@
         <v>184</v>
       </c>
     </row>
-    <row r="44" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:18" x14ac:dyDescent="0.3">
       <c r="B44" t="s">
         <v>269</v>
       </c>
@@ -3711,7 +3723,7 @@
         <v>271</v>
       </c>
     </row>
-    <row r="45" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:18" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A45" t="s">
         <v>109</v>
       </c>
@@ -3755,12 +3767,12 @@
         <v>188</v>
       </c>
     </row>
-    <row r="46" spans="1:18" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:18" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B46" s="14" t="s">
         <v>189</v>
       </c>
     </row>
-    <row r="47" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:18" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B47" s="7" t="s">
         <v>8</v>
       </c>
@@ -3801,7 +3813,7 @@
       </c>
       <c r="R47" s="8"/>
     </row>
-    <row r="48" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A48" t="s">
         <v>191</v>
       </c>
@@ -3842,7 +3854,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="49" spans="2:18" x14ac:dyDescent="0.25">
+    <row r="49" spans="2:18" x14ac:dyDescent="0.3">
       <c r="B49" t="s">
         <v>194</v>
       </c>
@@ -3874,7 +3886,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="50" spans="2:18" x14ac:dyDescent="0.25">
+    <row r="50" spans="2:18" x14ac:dyDescent="0.3">
       <c r="B50" t="s">
         <v>194</v>
       </c>
@@ -3906,12 +3918,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="51" spans="2:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="51" spans="2:18" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="C51" s="20"/>
       <c r="L51" s="16"/>
       <c r="M51" s="16"/>
     </row>
-    <row r="52" spans="2:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="52" spans="2:18" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B52" s="18" t="s">
         <v>196</v>
       </c>
@@ -3923,7 +3935,7 @@
       <c r="M52" s="17"/>
       <c r="N52" s="22"/>
     </row>
-    <row r="53" spans="2:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="53" spans="2:18" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B53" s="7" t="s">
         <v>8</v>
       </c>
@@ -3957,7 +3969,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="54" spans="2:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="54" spans="2:18" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B54" t="s">
         <v>284</v>
       </c>
@@ -3989,7 +4001,7 @@
         <v>2.4999999999999998E-2</v>
       </c>
     </row>
-    <row r="55" spans="2:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="55" spans="2:18" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B55" t="s">
         <v>285</v>
       </c>
@@ -4006,15 +4018,15 @@
         <v>26</v>
       </c>
       <c r="K55" s="32">
-        <f t="shared" ref="K55:K70" si="8">I55/1000*$C$52</f>
+        <f t="shared" ref="K55:K72" si="8">I55/1000*$C$52</f>
         <v>0.77999999999999992</v>
       </c>
       <c r="L55" s="32">
-        <f t="shared" ref="L55:L70" si="9">K55</f>
+        <f t="shared" ref="L55:L72" si="9">K55</f>
         <v>0.77999999999999992</v>
       </c>
       <c r="M55" s="32">
-        <f t="shared" ref="M55:M70" si="10">K55</f>
+        <f t="shared" ref="M55:M72" si="10">K55</f>
         <v>0.77999999999999992</v>
       </c>
       <c r="N55" s="27">
@@ -4023,7 +4035,7 @@
       <c r="Q55" s="43"/>
       <c r="R55" s="43"/>
     </row>
-    <row r="56" spans="2:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="56" spans="2:18" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B56" t="s">
         <v>286</v>
       </c>
@@ -4056,7 +4068,7 @@
       </c>
       <c r="P56" s="43"/>
     </row>
-    <row r="57" spans="2:18" x14ac:dyDescent="0.25">
+    <row r="57" spans="2:18" x14ac:dyDescent="0.3">
       <c r="B57" t="s">
         <v>288</v>
       </c>
@@ -4088,7 +4100,7 @@
         <v>8.819444444444445E-2</v>
       </c>
     </row>
-    <row r="58" spans="2:18" x14ac:dyDescent="0.25">
+    <row r="58" spans="2:18" x14ac:dyDescent="0.3">
       <c r="B58" t="s">
         <v>287</v>
       </c>
@@ -4120,76 +4132,76 @@
         <v>9.0277777777777787E-3</v>
       </c>
     </row>
-    <row r="59" spans="2:18" x14ac:dyDescent="0.25">
+    <row r="59" spans="2:18" x14ac:dyDescent="0.3">
       <c r="B59" t="s">
-        <v>273</v>
+        <v>363</v>
       </c>
       <c r="C59" t="s">
-        <v>233</v>
+        <v>365</v>
       </c>
       <c r="D59" t="s">
-        <v>22</v>
+        <v>57</v>
       </c>
       <c r="H59">
         <v>1</v>
       </c>
       <c r="I59">
-        <v>3</v>
+        <v>13</v>
       </c>
       <c r="K59" s="32">
         <f t="shared" si="8"/>
-        <v>0.09</v>
+        <v>0.38999999999999996</v>
       </c>
       <c r="L59" s="32">
         <f t="shared" si="9"/>
-        <v>0.09</v>
+        <v>0.38999999999999996</v>
       </c>
       <c r="M59" s="32">
         <f t="shared" si="10"/>
-        <v>0.09</v>
+        <v>0.38999999999999996</v>
       </c>
       <c r="N59" s="27">
-        <v>7.6388888888888886E-3</v>
-      </c>
-    </row>
-    <row r="60" spans="2:18" x14ac:dyDescent="0.25">
+        <v>1.4583333333333332E-2</v>
+      </c>
+    </row>
+    <row r="60" spans="2:18" x14ac:dyDescent="0.3">
       <c r="B60" t="s">
-        <v>272</v>
+        <v>364</v>
       </c>
       <c r="C60" t="s">
-        <v>233</v>
+        <v>366</v>
       </c>
       <c r="D60" t="s">
-        <v>22</v>
+        <v>57</v>
       </c>
       <c r="H60">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="I60">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="K60" s="32">
         <f t="shared" si="8"/>
-        <v>0.09</v>
+        <v>0.12</v>
       </c>
       <c r="L60" s="32">
         <f t="shared" si="9"/>
-        <v>0.09</v>
+        <v>0.12</v>
       </c>
       <c r="M60" s="32">
         <f t="shared" si="10"/>
-        <v>0.09</v>
+        <v>0.12</v>
       </c>
       <c r="N60" s="27">
-        <v>7.6388888888888886E-3</v>
-      </c>
-    </row>
-    <row r="61" spans="2:18" x14ac:dyDescent="0.25">
+        <v>4.8611111111111112E-3</v>
+      </c>
+    </row>
+    <row r="61" spans="2:18" x14ac:dyDescent="0.3">
       <c r="B61" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="C61" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="D61" t="s">
         <v>22</v>
@@ -4213,15 +4225,15 @@
         <v>0.09</v>
       </c>
       <c r="N61" s="27">
-        <v>1.3194444444444444E-2</v>
-      </c>
-    </row>
-    <row r="62" spans="2:18" x14ac:dyDescent="0.25">
+        <v>7.6388888888888886E-3</v>
+      </c>
+    </row>
+    <row r="62" spans="2:18" x14ac:dyDescent="0.3">
       <c r="B62" t="s">
-        <v>275</v>
+        <v>272</v>
       </c>
       <c r="C62" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="D62" t="s">
         <v>22</v>
@@ -4245,15 +4257,15 @@
         <v>0.09</v>
       </c>
       <c r="N62" s="27">
-        <v>1.3194444444444444E-2</v>
-      </c>
-    </row>
-    <row r="63" spans="2:18" x14ac:dyDescent="0.25">
+        <v>7.6388888888888886E-3</v>
+      </c>
+    </row>
+    <row r="63" spans="2:18" x14ac:dyDescent="0.3">
       <c r="B63" t="s">
-        <v>276</v>
+        <v>274</v>
       </c>
       <c r="C63" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="D63" t="s">
         <v>22</v>
@@ -4262,62 +4274,62 @@
         <v>1</v>
       </c>
       <c r="I63">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="K63" s="32">
         <f t="shared" si="8"/>
-        <v>0.12</v>
+        <v>0.09</v>
       </c>
       <c r="L63" s="32">
         <f t="shared" si="9"/>
-        <v>0.12</v>
+        <v>0.09</v>
       </c>
       <c r="M63" s="32">
         <f t="shared" si="10"/>
-        <v>0.12</v>
+        <v>0.09</v>
       </c>
       <c r="N63" s="27">
-        <v>1.2499999999999999E-2</v>
-      </c>
-    </row>
-    <row r="64" spans="2:18" x14ac:dyDescent="0.25">
+        <v>1.3194444444444444E-2</v>
+      </c>
+    </row>
+    <row r="64" spans="2:18" x14ac:dyDescent="0.3">
       <c r="B64" t="s">
-        <v>282</v>
+        <v>275</v>
       </c>
       <c r="C64" t="s">
-        <v>236</v>
+        <v>234</v>
       </c>
       <c r="D64" t="s">
         <v>22</v>
       </c>
       <c r="H64">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="I64">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="K64" s="32">
         <f t="shared" si="8"/>
-        <v>0.03</v>
+        <v>0.09</v>
       </c>
       <c r="L64" s="32">
         <f t="shared" si="9"/>
-        <v>0.03</v>
+        <v>0.09</v>
       </c>
       <c r="M64" s="32">
         <f t="shared" si="10"/>
-        <v>0.03</v>
+        <v>0.09</v>
       </c>
       <c r="N64" s="27">
-        <v>1.3888888888888889E-3</v>
-      </c>
-    </row>
-    <row r="65" spans="1:15" x14ac:dyDescent="0.25">
+        <v>1.3194444444444444E-2</v>
+      </c>
+    </row>
+    <row r="65" spans="1:15" x14ac:dyDescent="0.3">
       <c r="B65" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="C65" t="s">
-        <v>237</v>
+        <v>235</v>
       </c>
       <c r="D65" t="s">
         <v>22</v>
@@ -4326,62 +4338,62 @@
         <v>1</v>
       </c>
       <c r="I65">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="K65" s="32">
         <f t="shared" si="8"/>
-        <v>0.15</v>
+        <v>0.12</v>
       </c>
       <c r="L65" s="32">
         <f t="shared" si="9"/>
-        <v>0.15</v>
+        <v>0.12</v>
       </c>
       <c r="M65" s="32">
         <f t="shared" si="10"/>
-        <v>0.15</v>
+        <v>0.12</v>
       </c>
       <c r="N65" s="27">
-        <v>2.9861111111111113E-2</v>
-      </c>
-    </row>
-    <row r="66" spans="1:15" x14ac:dyDescent="0.25">
+        <v>1.2499999999999999E-2</v>
+      </c>
+    </row>
+    <row r="66" spans="1:15" x14ac:dyDescent="0.3">
       <c r="B66" t="s">
-        <v>278</v>
+        <v>282</v>
       </c>
       <c r="C66" t="s">
-        <v>240</v>
+        <v>236</v>
       </c>
       <c r="D66" t="s">
         <v>22</v>
       </c>
       <c r="H66">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="I66">
-        <v>14</v>
+        <v>1</v>
       </c>
       <c r="K66" s="32">
         <f t="shared" si="8"/>
-        <v>0.42</v>
+        <v>0.03</v>
       </c>
       <c r="L66" s="32">
         <f t="shared" si="9"/>
-        <v>0.42</v>
+        <v>0.03</v>
       </c>
       <c r="M66" s="32">
         <f t="shared" si="10"/>
-        <v>0.42</v>
+        <v>0.03</v>
       </c>
       <c r="N66" s="27">
-        <v>4.027777777777778E-2</v>
-      </c>
-    </row>
-    <row r="67" spans="1:15" x14ac:dyDescent="0.25">
+        <v>1.3888888888888889E-3</v>
+      </c>
+    </row>
+    <row r="67" spans="1:15" x14ac:dyDescent="0.3">
       <c r="B67" t="s">
-        <v>279</v>
+        <v>277</v>
       </c>
       <c r="C67" t="s">
-        <v>241</v>
+        <v>237</v>
       </c>
       <c r="D67" t="s">
         <v>22</v>
@@ -4390,30 +4402,30 @@
         <v>1</v>
       </c>
       <c r="I67">
-        <v>26</v>
+        <v>5</v>
       </c>
       <c r="K67" s="32">
         <f t="shared" si="8"/>
-        <v>0.77999999999999992</v>
+        <v>0.15</v>
       </c>
       <c r="L67" s="32">
         <f t="shared" si="9"/>
-        <v>0.77999999999999992</v>
+        <v>0.15</v>
       </c>
       <c r="M67" s="32">
         <f t="shared" si="10"/>
-        <v>0.77999999999999992</v>
+        <v>0.15</v>
       </c>
       <c r="N67" s="27">
-        <v>8.6805555555555566E-2</v>
-      </c>
-    </row>
-    <row r="68" spans="1:15" x14ac:dyDescent="0.25">
+        <v>2.9861111111111113E-2</v>
+      </c>
+    </row>
+    <row r="68" spans="1:15" x14ac:dyDescent="0.3">
       <c r="B68" t="s">
-        <v>280</v>
+        <v>278</v>
       </c>
       <c r="C68" t="s">
-        <v>238</v>
+        <v>240</v>
       </c>
       <c r="D68" t="s">
         <v>22</v>
@@ -4422,30 +4434,30 @@
         <v>1</v>
       </c>
       <c r="I68">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="K68" s="32">
         <f t="shared" si="8"/>
-        <v>0.51</v>
+        <v>0.42</v>
       </c>
       <c r="L68" s="32">
         <f t="shared" si="9"/>
-        <v>0.51</v>
+        <v>0.42</v>
       </c>
       <c r="M68" s="32">
         <f t="shared" si="10"/>
-        <v>0.51</v>
+        <v>0.42</v>
       </c>
       <c r="N68" s="27">
-        <v>5.2083333333333336E-2</v>
-      </c>
-    </row>
-    <row r="69" spans="1:15" x14ac:dyDescent="0.25">
+        <v>4.027777777777778E-2</v>
+      </c>
+    </row>
+    <row r="69" spans="1:15" x14ac:dyDescent="0.3">
       <c r="B69" t="s">
-        <v>281</v>
+        <v>279</v>
       </c>
       <c r="C69" t="s">
-        <v>239</v>
+        <v>241</v>
       </c>
       <c r="D69" t="s">
         <v>22</v>
@@ -4454,30 +4466,30 @@
         <v>1</v>
       </c>
       <c r="I69">
-        <v>6</v>
+        <v>26</v>
       </c>
       <c r="K69" s="32">
         <f t="shared" si="8"/>
-        <v>0.18</v>
+        <v>0.77999999999999992</v>
       </c>
       <c r="L69" s="32">
         <f t="shared" si="9"/>
-        <v>0.18</v>
+        <v>0.77999999999999992</v>
       </c>
       <c r="M69" s="32">
         <f t="shared" si="10"/>
-        <v>0.18</v>
+        <v>0.77999999999999992</v>
       </c>
       <c r="N69" s="27">
-        <v>2.2916666666666669E-2</v>
-      </c>
-    </row>
-    <row r="70" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+        <v>8.6805555555555566E-2</v>
+      </c>
+    </row>
+    <row r="70" spans="1:15" x14ac:dyDescent="0.3">
       <c r="B70" t="s">
-        <v>283</v>
+        <v>280</v>
       </c>
       <c r="C70" t="s">
-        <v>242</v>
+        <v>238</v>
       </c>
       <c r="D70" t="s">
         <v>22</v>
@@ -4486,709 +4498,649 @@
         <v>1</v>
       </c>
       <c r="I70">
-        <v>22</v>
+        <v>17</v>
       </c>
       <c r="K70" s="32">
         <f t="shared" si="8"/>
-        <v>0.65999999999999992</v>
+        <v>0.51</v>
       </c>
       <c r="L70" s="32">
         <f t="shared" si="9"/>
-        <v>0.65999999999999992</v>
+        <v>0.51</v>
       </c>
       <c r="M70" s="32">
         <f t="shared" si="10"/>
+        <v>0.51</v>
+      </c>
+      <c r="N70" s="27">
+        <v>5.2083333333333336E-2</v>
+      </c>
+    </row>
+    <row r="71" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="B71" t="s">
+        <v>281</v>
+      </c>
+      <c r="C71" t="s">
+        <v>239</v>
+      </c>
+      <c r="D71" t="s">
+        <v>22</v>
+      </c>
+      <c r="H71">
+        <v>1</v>
+      </c>
+      <c r="I71">
+        <v>6</v>
+      </c>
+      <c r="K71" s="32">
+        <f t="shared" si="8"/>
+        <v>0.18</v>
+      </c>
+      <c r="L71" s="32">
+        <f t="shared" si="9"/>
+        <v>0.18</v>
+      </c>
+      <c r="M71" s="32">
+        <f t="shared" si="10"/>
+        <v>0.18</v>
+      </c>
+      <c r="N71" s="27">
+        <v>2.2916666666666669E-2</v>
+      </c>
+    </row>
+    <row r="72" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B72" t="s">
+        <v>283</v>
+      </c>
+      <c r="C72" t="s">
+        <v>242</v>
+      </c>
+      <c r="D72" t="s">
+        <v>22</v>
+      </c>
+      <c r="H72">
+        <v>1</v>
+      </c>
+      <c r="I72">
+        <v>22</v>
+      </c>
+      <c r="K72" s="32">
+        <f t="shared" si="8"/>
         <v>0.65999999999999992</v>
       </c>
-      <c r="N70" s="27">
+      <c r="L72" s="32">
+        <f t="shared" si="9"/>
+        <v>0.65999999999999992</v>
+      </c>
+      <c r="M72" s="32">
+        <f t="shared" si="10"/>
+        <v>0.65999999999999992</v>
+      </c>
+      <c r="N72" s="27">
         <v>0.10208333333333335</v>
       </c>
     </row>
-    <row r="71" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B71" s="28" t="s">
+    <row r="73" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B73" s="28" t="s">
         <v>200</v>
       </c>
-      <c r="C71" s="10"/>
-      <c r="D71" s="10"/>
-      <c r="E71" s="10"/>
-      <c r="F71" s="10"/>
-      <c r="G71" s="10"/>
-      <c r="H71" s="10"/>
-      <c r="I71" s="10"/>
-      <c r="J71" s="10"/>
-      <c r="K71" s="10"/>
-      <c r="L71" s="10"/>
-      <c r="M71" s="10"/>
-      <c r="N71" s="10"/>
-      <c r="O71" s="10"/>
-    </row>
-    <row r="72" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B72" s="21" t="s">
+      <c r="C73" s="10"/>
+      <c r="D73" s="10"/>
+      <c r="E73" s="10"/>
+      <c r="F73" s="10"/>
+      <c r="G73" s="10"/>
+      <c r="H73" s="10"/>
+      <c r="I73" s="10"/>
+      <c r="J73" s="10"/>
+      <c r="K73" s="10"/>
+      <c r="L73" s="10"/>
+      <c r="M73" s="10"/>
+      <c r="N73" s="10"/>
+      <c r="O73" s="10"/>
+    </row>
+    <row r="74" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B74" s="21" t="s">
         <v>8</v>
       </c>
-      <c r="C72" s="21" t="s">
+      <c r="C74" s="21" t="s">
         <v>9</v>
       </c>
-      <c r="D72" s="29"/>
-      <c r="E72" s="29" t="s">
+      <c r="D74" s="29"/>
+      <c r="E74" s="29" t="s">
         <v>10</v>
       </c>
-      <c r="F72" s="29" t="s">
+      <c r="F74" s="29" t="s">
         <v>11</v>
       </c>
-      <c r="G72" s="29"/>
-    </row>
-    <row r="73" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="B73" s="31" t="s">
+      <c r="G74" s="29"/>
+    </row>
+    <row r="75" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="B75" s="31" t="s">
         <v>21</v>
       </c>
-      <c r="C73" t="s">
+      <c r="C75" t="s">
         <v>307</v>
       </c>
-      <c r="E73" t="s">
+      <c r="E75" t="s">
         <v>23</v>
       </c>
-      <c r="F73" t="s">
+      <c r="F75" t="s">
         <v>201</v>
       </c>
-      <c r="G73" t="s">
+      <c r="G75" t="s">
         <v>202</v>
       </c>
-      <c r="H73">
-        <v>1</v>
-      </c>
-      <c r="I73">
-        <v>1</v>
-      </c>
-      <c r="J73">
-        <f t="shared" ref="J73:J75" si="11">IF(H73&gt;0,CEILING(H73/I73,1),0)</f>
-        <v>1</v>
-      </c>
-      <c r="K73" s="25">
+      <c r="H75">
+        <v>1</v>
+      </c>
+      <c r="I75">
+        <v>1</v>
+      </c>
+      <c r="J75">
+        <f t="shared" ref="J75:J77" si="11">IF(H75&gt;0,CEILING(H75/I75,1),0)</f>
+        <v>1</v>
+      </c>
+      <c r="K75" s="25">
         <v>8.6300000000000008</v>
       </c>
-      <c r="L73" s="41">
-        <f>IF(H73&gt;0,K73/I73*H73,0)</f>
+      <c r="L75" s="41">
+        <f>IF(H75&gt;0,K75/I75*H75,0)</f>
         <v>8.6300000000000008</v>
       </c>
-      <c r="M73" s="32">
-        <f t="shared" ref="M73:M79" si="12">J73*K73</f>
+      <c r="M75" s="32">
+        <f t="shared" ref="M75:M81" si="12">J75*K75</f>
         <v>8.6300000000000008</v>
       </c>
-      <c r="O73" s="33" t="s">
+      <c r="O75" s="33" t="s">
         <v>203</v>
       </c>
     </row>
-    <row r="74" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="B74" t="s">
+    <row r="76" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="B76" t="s">
         <v>27</v>
       </c>
-      <c r="C74" t="s">
+      <c r="C76" t="s">
         <v>310</v>
       </c>
-      <c r="E74" t="s">
+      <c r="E76" t="s">
         <v>23</v>
       </c>
-      <c r="F74" t="s">
+      <c r="F76" t="s">
         <v>201</v>
       </c>
-      <c r="G74" t="s">
+      <c r="G76" t="s">
         <v>204</v>
       </c>
-      <c r="H74">
-        <v>1</v>
-      </c>
-      <c r="I74">
-        <v>1</v>
-      </c>
-      <c r="J74">
-        <v>1</v>
-      </c>
-      <c r="K74" s="12">
+      <c r="H76">
+        <v>1</v>
+      </c>
+      <c r="I76">
+        <v>1</v>
+      </c>
+      <c r="J76">
+        <v>1</v>
+      </c>
+      <c r="K76" s="12">
         <v>18.13</v>
       </c>
-      <c r="L74" s="41">
-        <f t="shared" ref="L74:L84" si="13">IF(H74&gt;0,K74/I74*H74,0)</f>
+      <c r="L76" s="41">
+        <f t="shared" ref="L76:L86" si="13">IF(H76&gt;0,K76/I76*H76,0)</f>
         <v>18.13</v>
       </c>
-      <c r="M74" s="32">
+      <c r="M76" s="32">
         <f t="shared" si="12"/>
         <v>18.13</v>
       </c>
-      <c r="O74" s="33" t="s">
+      <c r="O76" s="33" t="s">
         <v>205</v>
       </c>
     </row>
-    <row r="75" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="B75" t="s">
+    <row r="77" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="B77" t="s">
         <v>30</v>
       </c>
-      <c r="C75" t="s">
+      <c r="C77" t="s">
         <v>311</v>
       </c>
-      <c r="E75" t="s">
+      <c r="E77" t="s">
         <v>23</v>
       </c>
-      <c r="F75" t="s">
+      <c r="F77" t="s">
         <v>201</v>
       </c>
-      <c r="G75" s="24" t="s">
+      <c r="G77" s="24" t="s">
         <v>206</v>
       </c>
-      <c r="H75">
-        <v>1</v>
-      </c>
-      <c r="I75">
-        <v>1</v>
-      </c>
-      <c r="J75">
+      <c r="H77">
+        <v>1</v>
+      </c>
+      <c r="I77">
+        <v>1</v>
+      </c>
+      <c r="J77">
         <f t="shared" si="11"/>
         <v>1</v>
       </c>
-      <c r="K75" s="12">
+      <c r="K77" s="12">
         <v>10.08</v>
       </c>
-      <c r="L75" s="41">
+      <c r="L77" s="41">
         <f t="shared" si="13"/>
         <v>10.08</v>
       </c>
-      <c r="M75" s="32">
+      <c r="M77" s="32">
         <f t="shared" si="12"/>
         <v>10.08</v>
       </c>
-      <c r="O75" s="33" t="s">
+      <c r="O77" s="33" t="s">
         <v>207</v>
       </c>
     </row>
-    <row r="76" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A76" t="s">
+    <row r="78" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A78" t="s">
         <v>55</v>
       </c>
-      <c r="B76" s="30" t="s">
+      <c r="B78" s="30" t="s">
         <v>56</v>
       </c>
-      <c r="C76" t="s">
+      <c r="C78" t="s">
         <v>208</v>
       </c>
-      <c r="E76" t="s">
+      <c r="E78" t="s">
         <v>23</v>
       </c>
-      <c r="F76" t="s">
+      <c r="F78" t="s">
         <v>201</v>
       </c>
-      <c r="G76" t="s">
+      <c r="G78" t="s">
         <v>209</v>
       </c>
-      <c r="H76">
-        <v>1</v>
-      </c>
-      <c r="I76">
-        <v>1</v>
-      </c>
-      <c r="J76">
-        <v>1</v>
-      </c>
-      <c r="K76" s="25">
+      <c r="H78">
+        <v>1</v>
+      </c>
+      <c r="I78">
+        <v>1</v>
+      </c>
+      <c r="J78">
+        <v>1</v>
+      </c>
+      <c r="K78" s="25">
         <v>1.38</v>
       </c>
-      <c r="L76" s="41">
+      <c r="L78" s="41">
         <f t="shared" si="13"/>
         <v>1.38</v>
       </c>
-      <c r="M76" s="32">
+      <c r="M78" s="32">
         <f t="shared" si="12"/>
         <v>1.38</v>
       </c>
-      <c r="O76" s="8" t="s">
+      <c r="O78" s="8" t="s">
         <v>248</v>
       </c>
     </row>
-    <row r="77" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A77" t="s">
+    <row r="79" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A79" t="s">
         <v>49</v>
       </c>
-      <c r="B77" t="s">
+      <c r="B79" t="s">
         <v>50</v>
       </c>
-      <c r="C77" t="s">
+      <c r="C79" t="s">
         <v>51</v>
       </c>
-      <c r="E77" t="s">
+      <c r="E79" t="s">
         <v>23</v>
       </c>
-      <c r="F77" t="s">
+      <c r="F79" t="s">
         <v>201</v>
       </c>
-      <c r="G77" s="38" t="s">
+      <c r="G79" s="38" t="s">
         <v>250</v>
       </c>
-      <c r="H77">
-        <v>1</v>
-      </c>
-      <c r="I77">
-        <v>1</v>
-      </c>
-      <c r="J77">
-        <v>1</v>
-      </c>
-      <c r="K77" s="25">
+      <c r="H79">
+        <v>1</v>
+      </c>
+      <c r="I79">
+        <v>1</v>
+      </c>
+      <c r="J79">
+        <v>1</v>
+      </c>
+      <c r="K79" s="25">
         <v>1.38</v>
       </c>
-      <c r="L77" s="41">
-        <f>IF(H77&gt;0,K77/I77*H77,0)</f>
+      <c r="L79" s="41">
+        <f>IF(H79&gt;0,K79/I79*H79,0)</f>
         <v>1.38</v>
       </c>
-      <c r="M77" s="32">
-        <f>J77*K77</f>
+      <c r="M79" s="32">
+        <f>J79*K79</f>
         <v>1.38</v>
       </c>
-      <c r="O77" s="8" t="s">
+      <c r="O79" s="8" t="s">
         <v>251</v>
       </c>
     </row>
-    <row r="78" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A78" t="s">
+    <row r="80" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A80" t="s">
         <v>49</v>
       </c>
-      <c r="B78" t="s">
+      <c r="B80" t="s">
         <v>50</v>
       </c>
-      <c r="C78" t="s">
+      <c r="C80" t="s">
         <v>51</v>
       </c>
-      <c r="E78" t="s">
+      <c r="E80" t="s">
         <v>52</v>
       </c>
-      <c r="F78" t="s">
+      <c r="F80" t="s">
         <v>210</v>
       </c>
-      <c r="H78">
-        <v>1</v>
-      </c>
-      <c r="I78">
-        <v>1</v>
-      </c>
-      <c r="J78">
-        <v>1</v>
-      </c>
-      <c r="K78" s="25">
+      <c r="H80">
+        <v>1</v>
+      </c>
+      <c r="I80">
+        <v>1</v>
+      </c>
+      <c r="J80">
+        <v>1</v>
+      </c>
+      <c r="K80" s="25">
         <v>1.95</v>
       </c>
-      <c r="L78" s="41">
+      <c r="L80" s="41">
         <f t="shared" si="13"/>
         <v>1.95</v>
       </c>
-      <c r="M78" s="32">
+      <c r="M80" s="32">
         <f t="shared" si="12"/>
         <v>1.95</v>
       </c>
-      <c r="O78" s="8" t="s">
+      <c r="O80" s="8" t="s">
         <v>249</v>
       </c>
     </row>
-    <row r="79" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="B79" t="s">
+    <row r="81" spans="1:33" x14ac:dyDescent="0.3">
+      <c r="B81" t="s">
         <v>211</v>
       </c>
-      <c r="C79" t="s">
+      <c r="C81" t="s">
         <v>138</v>
       </c>
-      <c r="E79" t="s">
+      <c r="E81" t="s">
         <v>212</v>
       </c>
-      <c r="F79" t="s">
+      <c r="F81" t="s">
         <v>24</v>
       </c>
-      <c r="G79" s="24" t="s">
+      <c r="G81" s="24" t="s">
         <v>213</v>
       </c>
-      <c r="H79">
-        <v>1</v>
-      </c>
-      <c r="I79">
-        <v>1</v>
-      </c>
-      <c r="J79">
-        <v>1</v>
-      </c>
-      <c r="K79" s="12">
+      <c r="H81">
+        <v>1</v>
+      </c>
+      <c r="I81">
+        <v>1</v>
+      </c>
+      <c r="J81">
+        <v>1</v>
+      </c>
+      <c r="K81" s="12">
         <v>0.72</v>
       </c>
-      <c r="L79" s="41">
+      <c r="L81" s="41">
         <f t="shared" si="13"/>
         <v>0.72</v>
       </c>
-      <c r="M79" s="32">
+      <c r="M81" s="32">
         <f t="shared" si="12"/>
         <v>0.72</v>
       </c>
-      <c r="O79" s="33" t="s">
+      <c r="O81" s="33" t="s">
         <v>214</v>
       </c>
     </row>
-    <row r="80" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="B80" t="s">
+    <row r="82" spans="1:33" x14ac:dyDescent="0.3">
+      <c r="B82" t="s">
         <v>64</v>
       </c>
-      <c r="C80" t="s">
+      <c r="C82" t="s">
         <v>65</v>
       </c>
-      <c r="E80" t="s">
+      <c r="E82" t="s">
         <v>52</v>
       </c>
-      <c r="F80" t="s">
+      <c r="F82" t="s">
         <v>201</v>
       </c>
-      <c r="G80" s="24" t="s">
+      <c r="G82" s="24" t="s">
         <v>215</v>
       </c>
-      <c r="H80">
-        <v>1</v>
-      </c>
-      <c r="I80">
-        <v>1</v>
-      </c>
-      <c r="J80">
-        <v>1</v>
-      </c>
-      <c r="K80" s="25">
+      <c r="H82">
+        <v>1</v>
+      </c>
+      <c r="I82">
+        <v>1</v>
+      </c>
+      <c r="J82">
+        <v>1</v>
+      </c>
+      <c r="K82" s="25">
         <v>2.83</v>
       </c>
-      <c r="L80" s="41">
+      <c r="L82" s="41">
         <f t="shared" si="13"/>
         <v>2.83</v>
       </c>
-      <c r="M80" s="32">
-        <f>J80*K80</f>
+      <c r="M82" s="32">
+        <f>J82*K82</f>
         <v>2.83</v>
       </c>
-      <c r="O80" t="s">
+      <c r="O82" t="s">
         <v>216</v>
       </c>
     </row>
-    <row r="81" spans="1:33" x14ac:dyDescent="0.25">
-      <c r="B81" t="s">
+    <row r="83" spans="1:33" x14ac:dyDescent="0.3">
+      <c r="B83" t="s">
         <v>217</v>
       </c>
-      <c r="C81" t="s">
+      <c r="C83" t="s">
         <v>70</v>
       </c>
-      <c r="E81" t="s">
+      <c r="E83" t="s">
         <v>71</v>
       </c>
-      <c r="F81" t="s">
+      <c r="F83" t="s">
         <v>201</v>
       </c>
-      <c r="G81" s="24" t="s">
+      <c r="G83" s="24" t="s">
         <v>218</v>
       </c>
-      <c r="H81">
+      <c r="H83">
         <v>2</v>
       </c>
-      <c r="I81">
-        <v>1</v>
-      </c>
-      <c r="J81">
+      <c r="I83">
+        <v>1</v>
+      </c>
+      <c r="J83">
         <v>2</v>
       </c>
-      <c r="K81" s="9">
+      <c r="K83" s="9">
         <v>1.46</v>
       </c>
-      <c r="L81" s="41">
+      <c r="L83" s="41">
         <f t="shared" si="13"/>
         <v>2.92</v>
       </c>
-      <c r="M81" s="32">
-        <f>J81*K81</f>
+      <c r="M83" s="32">
+        <f>J83*K83</f>
         <v>2.92</v>
       </c>
-      <c r="O81" t="s">
+      <c r="O83" t="s">
         <v>219</v>
       </c>
     </row>
-    <row r="82" spans="1:33" x14ac:dyDescent="0.25">
-      <c r="B82" t="s">
+    <row r="84" spans="1:33" x14ac:dyDescent="0.3">
+      <c r="B84" t="s">
         <v>75</v>
       </c>
-      <c r="C82" t="s">
+      <c r="C84" t="s">
         <v>76</v>
       </c>
-      <c r="E82" t="s">
+      <c r="E84" t="s">
         <v>220</v>
       </c>
-      <c r="F82" t="s">
+      <c r="F84" t="s">
         <v>201</v>
       </c>
-      <c r="G82" s="24" t="s">
+      <c r="G84" s="24" t="s">
         <v>221</v>
       </c>
-      <c r="H82">
-        <v>1</v>
-      </c>
-      <c r="I82">
-        <v>1</v>
-      </c>
-      <c r="J82">
-        <v>1</v>
-      </c>
-      <c r="K82" s="9">
+      <c r="H84">
+        <v>1</v>
+      </c>
+      <c r="I84">
+        <v>1</v>
+      </c>
+      <c r="J84">
+        <v>1</v>
+      </c>
+      <c r="K84" s="9">
         <v>5.34</v>
       </c>
-      <c r="L82" s="41">
+      <c r="L84" s="41">
         <f t="shared" si="13"/>
         <v>5.34</v>
       </c>
-      <c r="M82" s="35">
-        <f>J82*K82</f>
+      <c r="M84" s="35">
+        <f>J84*K84</f>
         <v>5.34</v>
       </c>
-      <c r="O82" s="8" t="s">
+      <c r="O84" s="8" t="s">
         <v>254</v>
       </c>
     </row>
-    <row r="83" spans="1:33" x14ac:dyDescent="0.25">
-      <c r="B83" t="s">
+    <row r="85" spans="1:33" x14ac:dyDescent="0.3">
+      <c r="B85" t="s">
         <v>75</v>
       </c>
-      <c r="C83" t="s">
+      <c r="C85" t="s">
         <v>76</v>
       </c>
-      <c r="E83" t="s">
+      <c r="E85" t="s">
         <v>257</v>
       </c>
-      <c r="F83" t="s">
+      <c r="F85" t="s">
         <v>24</v>
       </c>
-      <c r="G83" s="24" t="s">
+      <c r="G85" s="24" t="s">
         <v>258</v>
       </c>
-      <c r="H83">
-        <v>1</v>
-      </c>
-      <c r="I83">
-        <v>1</v>
-      </c>
-      <c r="J83">
-        <v>1</v>
-      </c>
-      <c r="K83" s="9">
+      <c r="H85">
+        <v>1</v>
+      </c>
+      <c r="I85">
+        <v>1</v>
+      </c>
+      <c r="J85">
+        <v>1</v>
+      </c>
+      <c r="K85" s="9">
         <v>6.4</v>
       </c>
-      <c r="L83" s="41">
-        <f>IF(H83&gt;0,K83/I83*H83,0)</f>
+      <c r="L85" s="41">
+        <f>IF(H85&gt;0,K85/I85*H85,0)</f>
         <v>6.4</v>
       </c>
-      <c r="M83" s="35">
-        <f>J83*K83</f>
+      <c r="M85" s="35">
+        <f>J85*K85</f>
         <v>6.4</v>
       </c>
-      <c r="O83" s="8"/>
-    </row>
-    <row r="84" spans="1:33" x14ac:dyDescent="0.25">
-      <c r="B84" t="s">
+      <c r="O85" s="8"/>
+    </row>
+    <row r="86" spans="1:33" x14ac:dyDescent="0.3">
+      <c r="B86" t="s">
         <v>90</v>
       </c>
-      <c r="C84" t="s">
+      <c r="C86" t="s">
         <v>90</v>
       </c>
-      <c r="E84" t="s">
+      <c r="E86" t="s">
         <v>91</v>
       </c>
-      <c r="F84" t="s">
+      <c r="F86" t="s">
         <v>201</v>
       </c>
-      <c r="G84" s="24" t="s">
+      <c r="G86" s="24" t="s">
         <v>222</v>
       </c>
-      <c r="H84">
+      <c r="H86">
         <v>3</v>
       </c>
-      <c r="I84">
-        <v>1</v>
-      </c>
-      <c r="J84">
+      <c r="I86">
+        <v>1</v>
+      </c>
+      <c r="J86">
         <v>3</v>
       </c>
-      <c r="K84" s="9">
+      <c r="K86" s="9">
         <v>2.31</v>
       </c>
-      <c r="L84" s="41">
+      <c r="L86" s="41">
         <f t="shared" si="13"/>
         <v>6.93</v>
       </c>
-      <c r="M84" s="35">
-        <f>J84*K84</f>
+      <c r="M86" s="35">
+        <f>J86*K86</f>
         <v>6.93</v>
       </c>
-      <c r="O84" s="8" t="s">
+      <c r="O86" s="8" t="s">
         <v>223</v>
       </c>
     </row>
-    <row r="85" spans="1:33" s="34" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A85"/>
-      <c r="B85" t="s">
-        <v>121</v>
-      </c>
-      <c r="C85" t="s">
-        <v>122</v>
-      </c>
-      <c r="D85"/>
-      <c r="E85" t="s">
-        <v>224</v>
-      </c>
-      <c r="F85" t="s">
-        <v>24</v>
-      </c>
-      <c r="G85" s="24" t="s">
-        <v>225</v>
-      </c>
-      <c r="H85">
-        <v>2</v>
-      </c>
-      <c r="I85">
-        <v>1</v>
-      </c>
-      <c r="J85">
-        <v>2</v>
-      </c>
-      <c r="K85" s="12">
-        <v>0.89</v>
-      </c>
-      <c r="L85" s="41">
-        <f>IF(H85&gt;0,K85/I85*H85,0)</f>
-        <v>1.78</v>
-      </c>
-      <c r="M85" s="32">
-        <f t="shared" ref="M85:M89" si="14">J85*K85</f>
-        <v>1.78</v>
-      </c>
-      <c r="N85"/>
-      <c r="O85" s="33" t="s">
-        <v>226</v>
-      </c>
-      <c r="P85"/>
-      <c r="Q85"/>
-      <c r="R85"/>
-      <c r="S85"/>
-      <c r="T85"/>
-      <c r="U85"/>
-      <c r="V85"/>
-      <c r="W85"/>
-      <c r="X85"/>
-      <c r="Y85"/>
-      <c r="Z85"/>
-      <c r="AA85"/>
-      <c r="AB85"/>
-      <c r="AC85"/>
-      <c r="AD85"/>
-      <c r="AE85"/>
-      <c r="AF85"/>
-      <c r="AG85"/>
-    </row>
-    <row r="86" spans="1:33" s="34" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A86"/>
-      <c r="B86" t="s">
-        <v>349</v>
-      </c>
-      <c r="C86" t="s">
-        <v>348</v>
-      </c>
-      <c r="D86" t="s">
-        <v>57</v>
-      </c>
-      <c r="E86" t="s">
-        <v>347</v>
-      </c>
-      <c r="F86" t="s">
-        <v>201</v>
-      </c>
-      <c r="G86" s="24"/>
-      <c r="H86">
-        <v>1</v>
-      </c>
-      <c r="I86" s="16">
-        <v>1</v>
-      </c>
-      <c r="J86">
-        <v>1</v>
-      </c>
-      <c r="K86" s="12">
-        <v>0.89</v>
-      </c>
-      <c r="L86" s="41">
-        <f>IF(H86&gt;0,K86/H86*I86,0)</f>
-        <v>0.89</v>
-      </c>
-      <c r="M86" s="32">
-        <f t="shared" si="14"/>
-        <v>0.89</v>
-      </c>
-      <c r="N86"/>
-      <c r="O86" s="33" t="s">
-        <v>346</v>
-      </c>
-      <c r="P86"/>
-      <c r="Q86"/>
-      <c r="R86"/>
-      <c r="S86"/>
-      <c r="T86"/>
-      <c r="U86"/>
-      <c r="V86"/>
-      <c r="W86"/>
-      <c r="X86"/>
-      <c r="Y86"/>
-      <c r="Z86"/>
-      <c r="AA86"/>
-      <c r="AB86"/>
-      <c r="AC86"/>
-      <c r="AD86"/>
-      <c r="AE86"/>
-      <c r="AF86"/>
-      <c r="AG86"/>
-    </row>
-    <row r="87" spans="1:33" s="34" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:33" s="34" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A87"/>
       <c r="B87" t="s">
-        <v>354</v>
+        <v>121</v>
       </c>
       <c r="C87" t="s">
-        <v>354</v>
-      </c>
-      <c r="D87" t="s">
-        <v>170</v>
-      </c>
+        <v>122</v>
+      </c>
+      <c r="D87"/>
       <c r="E87" t="s">
-        <v>355</v>
+        <v>224</v>
       </c>
       <c r="F87" t="s">
-        <v>201</v>
-      </c>
-      <c r="G87" s="54" t="s">
-        <v>356</v>
+        <v>24</v>
+      </c>
+      <c r="G87" s="24" t="s">
+        <v>225</v>
       </c>
       <c r="H87">
-        <v>6</v>
-      </c>
-      <c r="I87" s="16">
+        <v>2</v>
+      </c>
+      <c r="I87">
         <v>1</v>
       </c>
       <c r="J87">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="K87" s="12">
-        <v>8.5999999999999993E-2</v>
-      </c>
-      <c r="L87" s="52">
-        <f>IF(H87&gt;0,K87/H87*I87,0)</f>
-        <v>1.4333333333333332E-2</v>
-      </c>
-      <c r="M87" s="25">
-        <f t="shared" si="14"/>
-        <v>0.51600000000000001</v>
+        <v>0.89</v>
+      </c>
+      <c r="L87" s="41">
+        <f>IF(H87&gt;0,K87/I87*H87,0)</f>
+        <v>1.78</v>
+      </c>
+      <c r="M87" s="32">
+        <f t="shared" ref="M87:M91" si="14">J87*K87</f>
+        <v>1.78</v>
       </c>
       <c r="N87"/>
       <c r="O87" s="33" t="s">
-        <v>353</v>
+        <v>226</v>
       </c>
       <c r="P87"/>
       <c r="Q87"/>
@@ -5209,49 +5161,47 @@
       <c r="AF87"/>
       <c r="AG87"/>
     </row>
-    <row r="88" spans="1:33" s="34" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:33" s="34" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A88"/>
       <c r="B88" t="s">
-        <v>159</v>
+        <v>349</v>
       </c>
       <c r="C88" t="s">
-        <v>159</v>
+        <v>348</v>
       </c>
       <c r="D88" t="s">
-        <v>170</v>
+        <v>57</v>
       </c>
       <c r="E88" t="s">
-        <v>355</v>
+        <v>347</v>
       </c>
       <c r="F88" t="s">
-        <v>24</v>
-      </c>
-      <c r="G88" s="54" t="s">
-        <v>358</v>
-      </c>
+        <v>201</v>
+      </c>
+      <c r="G88" s="24"/>
       <c r="H88">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="I88" s="16">
         <v>1</v>
       </c>
       <c r="J88">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="K88" s="12">
-        <v>0.2</v>
-      </c>
-      <c r="L88" s="52">
+        <v>0.89</v>
+      </c>
+      <c r="L88" s="41">
         <f>IF(H88&gt;0,K88/H88*I88,0)</f>
-        <v>3.3333333333333333E-2</v>
-      </c>
-      <c r="M88" s="25">
+        <v>0.89</v>
+      </c>
+      <c r="M88" s="32">
         <f t="shared" si="14"/>
-        <v>1.2000000000000002</v>
+        <v>0.89</v>
       </c>
       <c r="N88"/>
       <c r="O88" s="33" t="s">
-        <v>357</v>
+        <v>346</v>
       </c>
       <c r="P88"/>
       <c r="Q88"/>
@@ -5272,48 +5222,50 @@
       <c r="AF88"/>
       <c r="AG88"/>
     </row>
-    <row r="89" spans="1:33" s="34" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:33" s="34" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A89"/>
       <c r="B89" t="s">
-        <v>359</v>
+        <v>354</v>
       </c>
       <c r="C89" t="s">
-        <v>360</v>
+        <v>354</v>
       </c>
       <c r="D89" t="s">
-        <v>57</v>
+        <v>170</v>
       </c>
       <c r="E89" t="s">
-        <v>212</v>
+        <v>355</v>
       </c>
       <c r="F89" t="s">
-        <v>24</v>
+        <v>201</v>
       </c>
       <c r="G89" s="54" t="s">
-        <v>361</v>
+        <v>356</v>
       </c>
       <c r="H89">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="I89" s="16">
         <v>1</v>
       </c>
       <c r="J89">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="K89" s="12">
-        <v>0.96</v>
+        <v>8.5999999999999993E-2</v>
       </c>
       <c r="L89" s="52">
         <f>IF(H89&gt;0,K89/H89*I89,0)</f>
-        <v>0.96</v>
+        <v>1.4333333333333332E-2</v>
       </c>
       <c r="M89" s="25">
         <f t="shared" si="14"/>
-        <v>0.96</v>
+        <v>0.51600000000000001</v>
       </c>
       <c r="N89"/>
-      <c r="O89" s="33"/>
+      <c r="O89" s="33" t="s">
+        <v>353</v>
+      </c>
       <c r="P89"/>
       <c r="Q89"/>
       <c r="R89"/>
@@ -5333,22 +5285,50 @@
       <c r="AF89"/>
       <c r="AG89"/>
     </row>
-    <row r="90" spans="1:33" s="34" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:33" s="34" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A90"/>
-      <c r="B90"/>
-      <c r="C90"/>
-      <c r="D90"/>
-      <c r="E90"/>
-      <c r="F90"/>
-      <c r="G90" s="54"/>
-      <c r="H90"/>
-      <c r="I90" s="16"/>
-      <c r="J90"/>
-      <c r="K90" s="12"/>
-      <c r="L90" s="52"/>
-      <c r="M90" s="25"/>
+      <c r="B90" t="s">
+        <v>159</v>
+      </c>
+      <c r="C90" t="s">
+        <v>159</v>
+      </c>
+      <c r="D90" t="s">
+        <v>170</v>
+      </c>
+      <c r="E90" t="s">
+        <v>355</v>
+      </c>
+      <c r="F90" t="s">
+        <v>24</v>
+      </c>
+      <c r="G90" s="54" t="s">
+        <v>358</v>
+      </c>
+      <c r="H90">
+        <v>6</v>
+      </c>
+      <c r="I90" s="16">
+        <v>1</v>
+      </c>
+      <c r="J90">
+        <v>6</v>
+      </c>
+      <c r="K90" s="12">
+        <v>0.2</v>
+      </c>
+      <c r="L90" s="52">
+        <f>IF(H90&gt;0,K90/H90*I90,0)</f>
+        <v>3.3333333333333333E-2</v>
+      </c>
+      <c r="M90" s="25">
+        <f t="shared" si="14"/>
+        <v>1.2000000000000002</v>
+      </c>
       <c r="N90"/>
-      <c r="O90" s="33"/>
+      <c r="O90" s="33" t="s">
+        <v>357</v>
+      </c>
       <c r="P90"/>
       <c r="Q90"/>
       <c r="R90"/>
@@ -5368,20 +5348,46 @@
       <c r="AF90"/>
       <c r="AG90"/>
     </row>
-    <row r="91" spans="1:33" s="34" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:33" s="34" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A91"/>
-      <c r="B91"/>
-      <c r="C91"/>
-      <c r="D91"/>
-      <c r="E91"/>
-      <c r="F91"/>
-      <c r="G91" s="54"/>
-      <c r="H91"/>
-      <c r="I91" s="16"/>
-      <c r="J91"/>
-      <c r="K91" s="12"/>
-      <c r="L91" s="52"/>
-      <c r="M91" s="25"/>
+      <c r="B91" t="s">
+        <v>359</v>
+      </c>
+      <c r="C91" t="s">
+        <v>360</v>
+      </c>
+      <c r="D91" t="s">
+        <v>57</v>
+      </c>
+      <c r="E91" t="s">
+        <v>212</v>
+      </c>
+      <c r="F91" t="s">
+        <v>24</v>
+      </c>
+      <c r="G91" s="54" t="s">
+        <v>361</v>
+      </c>
+      <c r="H91">
+        <v>1</v>
+      </c>
+      <c r="I91" s="16">
+        <v>1</v>
+      </c>
+      <c r="J91">
+        <v>1</v>
+      </c>
+      <c r="K91" s="12">
+        <v>0.96</v>
+      </c>
+      <c r="L91" s="52">
+        <f>IF(H91&gt;0,K91/H91*I91,0)</f>
+        <v>0.96</v>
+      </c>
+      <c r="M91" s="25">
+        <f t="shared" si="14"/>
+        <v>0.96</v>
+      </c>
       <c r="N91"/>
       <c r="O91" s="33"/>
       <c r="P91"/>
@@ -5403,261 +5409,249 @@
       <c r="AF91"/>
       <c r="AG91"/>
     </row>
-    <row r="93" spans="1:33" x14ac:dyDescent="0.25">
-      <c r="B93" t="s">
+    <row r="92" spans="1:33" s="34" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A92"/>
+      <c r="B92"/>
+      <c r="C92"/>
+      <c r="D92"/>
+      <c r="E92"/>
+      <c r="F92"/>
+      <c r="G92" s="54"/>
+      <c r="H92"/>
+      <c r="I92" s="16"/>
+      <c r="J92"/>
+      <c r="K92" s="12"/>
+      <c r="L92" s="52"/>
+      <c r="M92" s="25"/>
+      <c r="N92"/>
+      <c r="O92" s="33"/>
+      <c r="P92"/>
+      <c r="Q92"/>
+      <c r="R92"/>
+      <c r="S92"/>
+      <c r="T92"/>
+      <c r="U92"/>
+      <c r="V92"/>
+      <c r="W92"/>
+      <c r="X92"/>
+      <c r="Y92"/>
+      <c r="Z92"/>
+      <c r="AA92"/>
+      <c r="AB92"/>
+      <c r="AC92"/>
+      <c r="AD92"/>
+      <c r="AE92"/>
+      <c r="AF92"/>
+      <c r="AG92"/>
+    </row>
+    <row r="93" spans="1:33" s="34" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A93"/>
+      <c r="B93"/>
+      <c r="C93"/>
+      <c r="D93"/>
+      <c r="E93"/>
+      <c r="F93"/>
+      <c r="G93" s="54"/>
+      <c r="H93"/>
+      <c r="I93" s="16"/>
+      <c r="J93"/>
+      <c r="K93" s="12"/>
+      <c r="L93" s="52"/>
+      <c r="M93" s="25"/>
+      <c r="N93"/>
+      <c r="O93" s="33"/>
+      <c r="P93"/>
+      <c r="Q93"/>
+      <c r="R93"/>
+      <c r="S93"/>
+      <c r="T93"/>
+      <c r="U93"/>
+      <c r="V93"/>
+      <c r="W93"/>
+      <c r="X93"/>
+      <c r="Y93"/>
+      <c r="Z93"/>
+      <c r="AA93"/>
+      <c r="AB93"/>
+      <c r="AC93"/>
+      <c r="AD93"/>
+      <c r="AE93"/>
+      <c r="AF93"/>
+      <c r="AG93"/>
+    </row>
+    <row r="95" spans="1:33" x14ac:dyDescent="0.3">
+      <c r="B95" t="s">
         <v>227</v>
       </c>
-      <c r="F93" t="s">
+      <c r="F95" t="s">
         <v>201</v>
       </c>
-      <c r="H93">
-        <v>1</v>
-      </c>
-      <c r="I93">
-        <v>1</v>
-      </c>
-      <c r="J93">
-        <f t="shared" ref="J93" si="15">IF(H93&gt;0,CEILING(H93/I93,1),0)</f>
-        <v>1</v>
-      </c>
-      <c r="K93" s="25">
+      <c r="H95">
+        <v>1</v>
+      </c>
+      <c r="I95">
+        <v>1</v>
+      </c>
+      <c r="J95">
+        <f t="shared" ref="J95" si="15">IF(H95&gt;0,CEILING(H95/I95,1),0)</f>
+        <v>1</v>
+      </c>
+      <c r="K95" s="25">
         <v>20</v>
       </c>
-      <c r="L93" s="32">
-        <f>IF(H93&gt;0,K93/I93,0)</f>
+      <c r="L95" s="32">
+        <f>IF(H95&gt;0,K95/I95,0)</f>
         <v>20</v>
       </c>
-      <c r="M93" s="32">
-        <f t="shared" ref="M93" si="16">J93*K93</f>
+      <c r="M95" s="32">
+        <f t="shared" ref="M95" si="16">J95*K95</f>
         <v>20</v>
       </c>
     </row>
-    <row r="95" spans="1:33" x14ac:dyDescent="0.25">
-      <c r="A95" t="s">
+    <row r="97" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A97" t="s">
         <v>20</v>
       </c>
-      <c r="B95" t="s">
+      <c r="B97" t="s">
         <v>21</v>
       </c>
-      <c r="C95" t="s">
+      <c r="C97" t="s">
         <v>307</v>
       </c>
-      <c r="D95" t="s">
+      <c r="D97" t="s">
         <v>22</v>
       </c>
-      <c r="E95" t="s">
+      <c r="E97" t="s">
         <v>23</v>
       </c>
-      <c r="F95" t="s">
+      <c r="F97" t="s">
         <v>23</v>
       </c>
-      <c r="G95" s="51">
+      <c r="G97" s="51">
         <v>4366</v>
       </c>
-      <c r="H95">
-        <v>1</v>
-      </c>
-      <c r="I95">
-        <v>1</v>
-      </c>
-      <c r="J95">
-        <f>IF(H95&gt;0,CEILING(H95/I95,1),0)</f>
-        <v>1</v>
-      </c>
-      <c r="K95" s="12"/>
-      <c r="L95" s="41">
-        <f t="shared" ref="L95:L97" si="17">IF(H95&gt;0,K95/I95*H95,0)</f>
+      <c r="H97">
+        <v>1</v>
+      </c>
+      <c r="I97">
+        <v>1</v>
+      </c>
+      <c r="J97">
+        <f>IF(H97&gt;0,CEILING(H97/I97,1),0)</f>
+        <v>1</v>
+      </c>
+      <c r="K97" s="12"/>
+      <c r="L97" s="41">
+        <f t="shared" ref="L97:L99" si="17">IF(H97&gt;0,K97/I97*H97,0)</f>
         <v>0</v>
       </c>
-      <c r="M95" s="41">
-        <f>J95*K95</f>
+      <c r="M97" s="41">
+        <f>J97*K97</f>
         <v>0</v>
       </c>
-      <c r="O95" s="33" t="s">
+      <c r="O97" s="33" t="s">
         <v>314</v>
       </c>
     </row>
-    <row r="96" spans="1:33" x14ac:dyDescent="0.25">
-      <c r="A96" t="s">
+    <row r="98" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A98" t="s">
         <v>26</v>
       </c>
-      <c r="B96" t="s">
+      <c r="B98" t="s">
         <v>27</v>
       </c>
-      <c r="C96" t="s">
+      <c r="C98" t="s">
         <v>310</v>
       </c>
-      <c r="D96" t="s">
+      <c r="D98" t="s">
         <v>22</v>
       </c>
-      <c r="E96" t="s">
+      <c r="E98" t="s">
         <v>23</v>
       </c>
-      <c r="F96" t="s">
+      <c r="F98" t="s">
         <v>23</v>
       </c>
-      <c r="G96" s="51">
+      <c r="G98" s="51">
         <v>4414</v>
       </c>
-      <c r="H96">
-        <v>1</v>
-      </c>
-      <c r="I96">
-        <v>1</v>
-      </c>
-      <c r="J96">
-        <f t="shared" ref="J96:J97" si="18">IF(H96&gt;0,CEILING(H96/I96,1),0)</f>
-        <v>1</v>
-      </c>
-      <c r="K96" s="12"/>
-      <c r="L96" s="41">
+      <c r="H98">
+        <v>1</v>
+      </c>
+      <c r="I98">
+        <v>1</v>
+      </c>
+      <c r="J98">
+        <f t="shared" ref="J98:J99" si="18">IF(H98&gt;0,CEILING(H98/I98,1),0)</f>
+        <v>1</v>
+      </c>
+      <c r="K98" s="12"/>
+      <c r="L98" s="41">
         <f t="shared" si="17"/>
         <v>0</v>
       </c>
-      <c r="M96" s="41">
-        <f t="shared" ref="M96:M97" si="19">J96*K96</f>
+      <c r="M98" s="41">
+        <f t="shared" ref="M98:M99" si="19">J98*K98</f>
         <v>0</v>
       </c>
-      <c r="O96" s="33" t="s">
+      <c r="O98" s="33" t="s">
         <v>313</v>
       </c>
     </row>
-    <row r="97" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A97" t="s">
+    <row r="99" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A99" t="s">
         <v>29</v>
       </c>
-      <c r="B97" t="s">
+      <c r="B99" t="s">
         <v>30</v>
       </c>
-      <c r="C97" t="s">
+      <c r="C99" t="s">
         <v>311</v>
       </c>
-      <c r="D97" t="s">
+      <c r="D99" t="s">
         <v>22</v>
       </c>
-      <c r="E97" t="s">
+      <c r="E99" t="s">
         <v>23</v>
       </c>
-      <c r="F97" t="s">
+      <c r="F99" t="s">
         <v>23</v>
       </c>
-      <c r="G97" s="51">
+      <c r="G99" s="51">
         <v>4633</v>
       </c>
-      <c r="H97">
-        <v>1</v>
-      </c>
-      <c r="I97">
-        <v>1</v>
-      </c>
-      <c r="J97">
+      <c r="H99">
+        <v>1</v>
+      </c>
+      <c r="I99">
+        <v>1</v>
+      </c>
+      <c r="J99">
         <f t="shared" si="18"/>
         <v>1</v>
       </c>
-      <c r="K97" s="12"/>
-      <c r="L97" s="41">
+      <c r="K99" s="12"/>
+      <c r="L99" s="41">
         <f t="shared" si="17"/>
         <v>0</v>
       </c>
-      <c r="M97" s="41">
+      <c r="M99" s="41">
         <f t="shared" si="19"/>
         <v>0</v>
       </c>
-      <c r="O97" s="33" t="s">
+      <c r="O99" s="33" t="s">
         <v>312</v>
       </c>
     </row>
-    <row r="98" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A98" t="s">
+    <row r="100" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A100" t="s">
         <v>49</v>
       </c>
-      <c r="B98" t="s">
+      <c r="B100" t="s">
         <v>50</v>
       </c>
-      <c r="C98" t="s">
+      <c r="C100" t="s">
         <v>51</v>
-      </c>
-      <c r="E98" t="s">
-        <v>23</v>
-      </c>
-      <c r="F98" t="s">
-        <v>23</v>
-      </c>
-      <c r="G98" s="51">
-        <v>4399</v>
-      </c>
-      <c r="H98">
-        <v>1</v>
-      </c>
-      <c r="I98">
-        <v>1</v>
-      </c>
-      <c r="J98">
-        <v>1</v>
-      </c>
-      <c r="K98" s="25"/>
-      <c r="L98" s="41">
-        <f>IF(H98&gt;0,K98/I98*H98,0)</f>
-        <v>0</v>
-      </c>
-      <c r="M98" s="32">
-        <f>J98*K98</f>
-        <v>0</v>
-      </c>
-      <c r="O98" s="8" t="s">
-        <v>316</v>
-      </c>
-    </row>
-    <row r="99" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A99" t="s">
-        <v>55</v>
-      </c>
-      <c r="B99" t="s">
-        <v>56</v>
-      </c>
-      <c r="C99" t="s">
-        <v>208</v>
-      </c>
-      <c r="E99" t="s">
-        <v>23</v>
-      </c>
-      <c r="F99" t="s">
-        <v>23</v>
-      </c>
-      <c r="G99">
-        <v>4210</v>
-      </c>
-      <c r="H99">
-        <v>1</v>
-      </c>
-      <c r="I99">
-        <v>1</v>
-      </c>
-      <c r="J99">
-        <v>1</v>
-      </c>
-      <c r="K99" s="25"/>
-      <c r="L99" s="41">
-        <f>IF(H99&gt;0,K99/I99*H99,0)</f>
-        <v>0</v>
-      </c>
-      <c r="M99" s="32">
-        <f>J99*K99</f>
-        <v>0</v>
-      </c>
-      <c r="O99" s="8" t="s">
-        <v>315</v>
-      </c>
-    </row>
-    <row r="100" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A100" t="s">
-        <v>44</v>
-      </c>
-      <c r="B100" t="s">
-        <v>318</v>
-      </c>
-      <c r="C100" t="s">
-        <v>326</v>
       </c>
       <c r="E100" t="s">
         <v>23</v>
@@ -5665,8 +5659,8 @@
       <c r="F100" t="s">
         <v>23</v>
       </c>
-      <c r="G100">
-        <v>4209</v>
+      <c r="G100" s="51">
+        <v>4399</v>
       </c>
       <c r="H100">
         <v>1</v>
@@ -5677,6 +5671,7 @@
       <c r="J100">
         <v>1</v>
       </c>
+      <c r="K100" s="25"/>
       <c r="L100" s="41">
         <f>IF(H100&gt;0,K100/I100*H100,0)</f>
         <v>0</v>
@@ -5686,30 +5681,27 @@
         <v>0</v>
       </c>
       <c r="O100" s="8" t="s">
-        <v>317</v>
-      </c>
-    </row>
-    <row r="101" spans="1:15" x14ac:dyDescent="0.25">
+        <v>316</v>
+      </c>
+    </row>
+    <row r="101" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A101" t="s">
-        <v>110</v>
+        <v>55</v>
       </c>
       <c r="B101" t="s">
-        <v>111</v>
+        <v>56</v>
       </c>
       <c r="C101" t="s">
-        <v>320</v>
-      </c>
-      <c r="D101" t="s">
-        <v>57</v>
+        <v>208</v>
       </c>
       <c r="E101" t="s">
         <v>23</v>
       </c>
       <c r="F101" t="s">
-        <v>24</v>
-      </c>
-      <c r="G101" s="51">
-        <v>938</v>
+        <v>23</v>
+      </c>
+      <c r="G101">
+        <v>4210</v>
       </c>
       <c r="H101">
         <v>1</v>
@@ -5717,32 +5709,31 @@
       <c r="I101">
         <v>1</v>
       </c>
-      <c r="J101" s="40">
-        <f t="shared" ref="J101" si="20">IF(H101&gt;0,CEILING(H101/I101,1),0)</f>
-        <v>1</v>
-      </c>
-      <c r="K101" s="12"/>
+      <c r="J101">
+        <v>1</v>
+      </c>
+      <c r="K101" s="25"/>
       <c r="L101" s="41">
-        <f t="shared" ref="L101" si="21">IF(H101&gt;0,K101/I101*H101,0)</f>
+        <f>IF(H101&gt;0,K101/I101*H101,0)</f>
         <v>0</v>
       </c>
-      <c r="M101" s="41">
-        <f t="shared" ref="M101" si="22">J101*K101</f>
+      <c r="M101" s="32">
+        <f>J101*K101</f>
         <v>0</v>
       </c>
-      <c r="O101" s="33" t="s">
-        <v>321</v>
-      </c>
-    </row>
-    <row r="102" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="O101" s="8" t="s">
+        <v>315</v>
+      </c>
+    </row>
+    <row r="102" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A102" t="s">
+        <v>44</v>
+      </c>
       <c r="B102" t="s">
-        <v>351</v>
-      </c>
-      <c r="C102" s="53" t="s">
-        <v>352</v>
-      </c>
-      <c r="D102" t="s">
-        <v>57</v>
+        <v>318</v>
+      </c>
+      <c r="C102" t="s">
+        <v>326</v>
       </c>
       <c r="E102" t="s">
         <v>23</v>
@@ -5750,440 +5741,525 @@
       <c r="F102" t="s">
         <v>23</v>
       </c>
-      <c r="G102" s="51">
+      <c r="G102">
+        <v>4209</v>
+      </c>
+      <c r="H102">
+        <v>1</v>
+      </c>
+      <c r="I102">
+        <v>1</v>
+      </c>
+      <c r="J102">
+        <v>1</v>
+      </c>
+      <c r="L102" s="41">
+        <f>IF(H102&gt;0,K102/I102*H102,0)</f>
+        <v>0</v>
+      </c>
+      <c r="M102" s="32">
+        <f>J102*K102</f>
+        <v>0</v>
+      </c>
+      <c r="O102" s="8" t="s">
+        <v>317</v>
+      </c>
+    </row>
+    <row r="103" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A103" t="s">
+        <v>110</v>
+      </c>
+      <c r="B103" t="s">
+        <v>111</v>
+      </c>
+      <c r="C103" t="s">
+        <v>320</v>
+      </c>
+      <c r="D103" t="s">
+        <v>57</v>
+      </c>
+      <c r="E103" t="s">
+        <v>23</v>
+      </c>
+      <c r="F103" t="s">
+        <v>24</v>
+      </c>
+      <c r="G103" s="51">
+        <v>938</v>
+      </c>
+      <c r="H103">
+        <v>1</v>
+      </c>
+      <c r="I103">
+        <v>1</v>
+      </c>
+      <c r="J103" s="40">
+        <f t="shared" ref="J103" si="20">IF(H103&gt;0,CEILING(H103/I103,1),0)</f>
+        <v>1</v>
+      </c>
+      <c r="K103" s="12"/>
+      <c r="L103" s="41">
+        <f t="shared" ref="L103" si="21">IF(H103&gt;0,K103/I103*H103,0)</f>
+        <v>0</v>
+      </c>
+      <c r="M103" s="41">
+        <f t="shared" ref="M103" si="22">J103*K103</f>
+        <v>0</v>
+      </c>
+      <c r="O103" s="33" t="s">
+        <v>321</v>
+      </c>
+    </row>
+    <row r="104" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="B104" t="s">
+        <v>351</v>
+      </c>
+      <c r="C104" s="53" t="s">
+        <v>352</v>
+      </c>
+      <c r="D104" t="s">
+        <v>57</v>
+      </c>
+      <c r="E104" t="s">
+        <v>23</v>
+      </c>
+      <c r="F104" t="s">
+        <v>23</v>
+      </c>
+      <c r="G104" s="51">
         <v>1119</v>
       </c>
-      <c r="H102">
+      <c r="H104">
         <v>2</v>
       </c>
-      <c r="I102">
+      <c r="I104">
         <v>10</v>
       </c>
-      <c r="J102" s="40">
-        <v>1</v>
-      </c>
-      <c r="K102" s="12"/>
-      <c r="L102" s="41">
-        <f t="shared" ref="L102:L103" si="23">IF(H102&gt;0,K102/I102*H102,0)</f>
+      <c r="J104" s="40">
+        <v>1</v>
+      </c>
+      <c r="K104" s="12"/>
+      <c r="L104" s="41">
+        <f t="shared" ref="L104:L105" si="23">IF(H104&gt;0,K104/I104*H104,0)</f>
         <v>0</v>
       </c>
-      <c r="M102" s="41">
-        <f t="shared" ref="M102:M103" si="24">J102*K102</f>
+      <c r="M104" s="41">
+        <f t="shared" ref="M104:M105" si="24">J104*K104</f>
         <v>0</v>
       </c>
-      <c r="O102" s="33" t="s">
+      <c r="O104" s="33" t="s">
         <v>350</v>
       </c>
     </row>
-    <row r="103" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="C103" s="53"/>
-      <c r="G103" s="51"/>
-      <c r="J103" s="40"/>
-      <c r="K103" s="12"/>
-      <c r="L103" s="52">
+    <row r="105" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="C105" s="53"/>
+      <c r="G105" s="51"/>
+      <c r="J105" s="40"/>
+      <c r="K105" s="12"/>
+      <c r="L105" s="52">
         <f t="shared" si="23"/>
         <v>0</v>
       </c>
-      <c r="M103" s="52">
+      <c r="M105" s="52">
         <f t="shared" si="24"/>
         <v>0</v>
       </c>
-      <c r="O103" s="33"/>
-    </row>
-    <row r="105" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A105" t="s">
+      <c r="O105" s="33"/>
+    </row>
+    <row r="107" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A107" t="s">
         <v>63</v>
       </c>
-      <c r="B105" t="s">
+      <c r="B107" t="s">
         <v>64</v>
       </c>
-      <c r="C105" t="s">
+      <c r="C107" t="s">
         <v>65</v>
       </c>
-      <c r="D105" t="s">
+      <c r="D107" t="s">
         <v>22</v>
       </c>
-      <c r="E105" t="s">
+      <c r="E107" t="s">
         <v>52</v>
       </c>
-      <c r="F105" t="s">
+      <c r="F107" t="s">
         <v>323</v>
       </c>
-      <c r="G105" s="24"/>
-      <c r="H105">
-        <v>1</v>
-      </c>
-      <c r="I105">
+      <c r="G107" s="24"/>
+      <c r="H107">
+        <v>1</v>
+      </c>
+      <c r="I107">
         <v>2</v>
       </c>
-      <c r="J105" s="40">
-        <f t="shared" ref="J105:J115" si="25">IF(H105&gt;0,CEILING(H105/I105,1),0)</f>
-        <v>1</v>
-      </c>
-      <c r="K105" s="12"/>
-      <c r="L105" s="41">
-        <f t="shared" ref="L105:L115" si="26">IF(H105&gt;0,K105/I105*H105,0)</f>
+      <c r="J107" s="40">
+        <f t="shared" ref="J107:J117" si="25">IF(H107&gt;0,CEILING(H107/I107,1),0)</f>
+        <v>1</v>
+      </c>
+      <c r="K107" s="12"/>
+      <c r="L107" s="41">
+        <f t="shared" ref="L107:L117" si="26">IF(H107&gt;0,K107/I107*H107,0)</f>
         <v>0</v>
       </c>
-      <c r="M105" s="41">
-        <f t="shared" ref="M105:M115" si="27">J105*K105</f>
+      <c r="M107" s="41">
+        <f t="shared" ref="M107:M117" si="27">J107*K107</f>
         <v>0</v>
       </c>
-      <c r="O105" s="33" t="s">
+      <c r="O107" s="33" t="s">
         <v>322</v>
       </c>
     </row>
-    <row r="106" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A106" t="s">
+    <row r="108" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A108" t="s">
         <v>142</v>
       </c>
-      <c r="B106" t="s">
+      <c r="B108" t="s">
         <v>143</v>
       </c>
-      <c r="C106" t="s">
+      <c r="C108" t="s">
         <v>144</v>
       </c>
-      <c r="D106" t="s">
+      <c r="D108" t="s">
         <v>57</v>
       </c>
-      <c r="E106" t="s">
+      <c r="E108" t="s">
         <v>52</v>
       </c>
-      <c r="F106" t="s">
+      <c r="F108" t="s">
         <v>323</v>
       </c>
-      <c r="G106" s="24" t="s">
+      <c r="G108" s="24" t="s">
         <v>325</v>
       </c>
-      <c r="H106">
-        <v>1</v>
-      </c>
-      <c r="I106">
-        <v>1</v>
-      </c>
-      <c r="J106" s="40">
+      <c r="H108">
+        <v>1</v>
+      </c>
+      <c r="I108">
+        <v>1</v>
+      </c>
+      <c r="J108" s="40">
         <f t="shared" si="25"/>
         <v>1</v>
       </c>
-      <c r="K106" s="12"/>
-      <c r="L106" s="41">
+      <c r="K108" s="12"/>
+      <c r="L108" s="41">
         <f t="shared" si="26"/>
         <v>0</v>
       </c>
-      <c r="M106" s="41">
+      <c r="M108" s="41">
         <f t="shared" si="27"/>
         <v>0</v>
       </c>
-      <c r="O106" s="33" t="s">
+      <c r="O108" s="33" t="s">
         <v>324</v>
       </c>
     </row>
-    <row r="107" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="J107" s="40">
+    <row r="109" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="J109" s="40">
         <f t="shared" si="25"/>
         <v>0</v>
       </c>
-      <c r="L107" s="41">
+      <c r="L109" s="41">
         <f t="shared" si="26"/>
         <v>0</v>
       </c>
-      <c r="M107" s="41">
+      <c r="M109" s="41">
         <f t="shared" si="27"/>
         <v>0</v>
       </c>
     </row>
-    <row r="108" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="B108" t="s">
+    <row r="110" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="B110" t="s">
         <v>333</v>
       </c>
-      <c r="C108" t="s">
+      <c r="C110" t="s">
         <v>327</v>
       </c>
-      <c r="D108" t="s">
+      <c r="D110" t="s">
         <v>264</v>
       </c>
-      <c r="E108" t="s">
+      <c r="E110" t="s">
         <v>334</v>
       </c>
-      <c r="F108" t="s">
+      <c r="F110" t="s">
         <v>149</v>
       </c>
-      <c r="H108">
+      <c r="H110">
         <v>6</v>
       </c>
-      <c r="I108">
+      <c r="I110">
         <v>100</v>
       </c>
-      <c r="J108" s="40">
+      <c r="J110" s="40">
         <f t="shared" si="25"/>
         <v>1</v>
       </c>
-      <c r="K108">
+      <c r="K110">
         <v>43.31</v>
       </c>
-      <c r="L108" s="41">
+      <c r="L110" s="41">
         <f t="shared" si="26"/>
         <v>2.5986000000000002</v>
       </c>
-      <c r="M108" s="41">
+      <c r="M110" s="41">
         <f t="shared" si="27"/>
         <v>43.31</v>
       </c>
-      <c r="O108" t="s">
+      <c r="O110" t="s">
         <v>332</v>
       </c>
     </row>
-    <row r="109" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="B109" t="s">
+    <row r="111" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="B111" t="s">
         <v>295</v>
       </c>
-      <c r="C109" t="s">
+      <c r="C111" t="s">
         <v>295</v>
       </c>
-      <c r="D109" t="s">
+      <c r="D111" t="s">
         <v>264</v>
       </c>
-      <c r="E109" t="s">
+      <c r="E111" t="s">
         <v>341</v>
       </c>
-      <c r="F109" t="s">
+      <c r="F111" t="s">
         <v>149</v>
       </c>
-      <c r="H109">
+      <c r="H111">
         <v>2</v>
       </c>
-      <c r="I109">
+      <c r="I111">
         <v>12</v>
       </c>
-      <c r="J109" s="40">
+      <c r="J111" s="40">
         <f t="shared" si="25"/>
         <v>1</v>
       </c>
-      <c r="K109">
+      <c r="K111">
         <v>13.99</v>
       </c>
-      <c r="L109" s="41">
+      <c r="L111" s="41">
         <f t="shared" si="26"/>
         <v>2.3316666666666666</v>
       </c>
-      <c r="M109" s="41">
+      <c r="M111" s="41">
         <f t="shared" si="27"/>
         <v>13.99</v>
       </c>
-      <c r="O109" t="s">
+      <c r="O111" t="s">
         <v>340</v>
       </c>
     </row>
-    <row r="110" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="B110" t="s">
+    <row r="112" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="B112" t="s">
         <v>328</v>
       </c>
-      <c r="C110" t="s">
+      <c r="C112" t="s">
         <v>328</v>
       </c>
-      <c r="D110" t="s">
+      <c r="D112" t="s">
         <v>264</v>
       </c>
-      <c r="E110" t="s">
+      <c r="E112" t="s">
         <v>336</v>
       </c>
-      <c r="F110" t="s">
+      <c r="F112" t="s">
         <v>149</v>
       </c>
-      <c r="H110">
+      <c r="H112">
         <v>3</v>
       </c>
-      <c r="I110">
+      <c r="I112">
         <v>500</v>
       </c>
-      <c r="J110" s="40">
+      <c r="J112" s="40">
         <f t="shared" si="25"/>
         <v>1</v>
       </c>
-      <c r="K110">
+      <c r="K112">
         <v>16.36</v>
       </c>
-      <c r="L110" s="41">
+      <c r="L112" s="41">
         <f t="shared" si="26"/>
         <v>9.8159999999999997E-2</v>
       </c>
-      <c r="M110" s="41">
+      <c r="M112" s="41">
         <f t="shared" si="27"/>
         <v>16.36</v>
       </c>
-      <c r="O110" t="s">
+      <c r="O112" t="s">
         <v>335</v>
       </c>
     </row>
-    <row r="111" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="B111" t="s">
+    <row r="113" spans="2:15" x14ac:dyDescent="0.3">
+      <c r="B113" t="s">
         <v>338</v>
       </c>
-      <c r="C111" t="s">
+      <c r="C113" t="s">
         <v>329</v>
       </c>
-      <c r="D111" t="s">
+      <c r="D113" t="s">
         <v>264</v>
       </c>
-      <c r="E111" t="s">
+      <c r="E113" t="s">
         <v>339</v>
       </c>
-      <c r="F111" t="s">
+      <c r="F113" t="s">
         <v>149</v>
       </c>
-      <c r="H111">
+      <c r="H113">
         <v>2</v>
       </c>
-      <c r="I111">
+      <c r="I113">
         <v>100</v>
       </c>
-      <c r="J111" s="40">
+      <c r="J113" s="40">
         <f t="shared" si="25"/>
         <v>1</v>
       </c>
-      <c r="K111">
+      <c r="K113">
         <v>15.51</v>
       </c>
-      <c r="L111" s="41">
+      <c r="L113" s="41">
         <f t="shared" si="26"/>
         <v>0.31019999999999998</v>
       </c>
-      <c r="M111" s="41">
+      <c r="M113" s="41">
         <f t="shared" si="27"/>
         <v>15.51</v>
       </c>
-      <c r="O111" t="s">
+      <c r="O113" t="s">
         <v>337</v>
       </c>
     </row>
-    <row r="112" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="B112" t="s">
+    <row r="114" spans="2:15" x14ac:dyDescent="0.3">
+      <c r="B114" t="s">
         <v>269</v>
       </c>
-      <c r="C112" t="s">
+      <c r="C114" t="s">
         <v>330</v>
       </c>
-      <c r="D112" t="s">
+      <c r="D114" t="s">
         <v>264</v>
       </c>
-      <c r="F112" t="s">
+      <c r="F114" t="s">
         <v>149</v>
       </c>
-      <c r="H112">
+      <c r="H114">
         <v>6</v>
       </c>
-      <c r="I112">
+      <c r="I114">
         <v>100</v>
       </c>
-      <c r="J112" s="40">
+      <c r="J114" s="40">
         <f t="shared" si="25"/>
         <v>1</v>
       </c>
-      <c r="K112">
+      <c r="K114">
         <v>19.489999999999998</v>
       </c>
-      <c r="L112" s="41">
+      <c r="L114" s="41">
         <f t="shared" si="26"/>
         <v>1.1694</v>
       </c>
-      <c r="M112" s="41">
+      <c r="M114" s="41">
         <f t="shared" si="27"/>
         <v>19.489999999999998</v>
       </c>
-      <c r="O112" t="s">
+      <c r="O114" t="s">
         <v>342</v>
       </c>
     </row>
-    <row r="113" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B113" t="s">
+    <row r="115" spans="2:15" x14ac:dyDescent="0.3">
+      <c r="B115" t="s">
         <v>345</v>
       </c>
-      <c r="C113" t="s">
+      <c r="C115" t="s">
         <v>331</v>
       </c>
-      <c r="D113" t="s">
+      <c r="D115" t="s">
         <v>264</v>
       </c>
-      <c r="E113" t="s">
+      <c r="E115" t="s">
         <v>344</v>
       </c>
-      <c r="F113" t="s">
+      <c r="F115" t="s">
         <v>149</v>
       </c>
-      <c r="H113">
-        <v>1</v>
-      </c>
-      <c r="I113">
+      <c r="H115">
+        <v>1</v>
+      </c>
+      <c r="I115">
         <v>10</v>
       </c>
-      <c r="J113" s="40">
+      <c r="J115" s="40">
         <f t="shared" si="25"/>
         <v>1</v>
       </c>
-      <c r="K113">
+      <c r="K115">
         <v>12.31</v>
       </c>
-      <c r="L113" s="41">
+      <c r="L115" s="41">
         <f t="shared" si="26"/>
         <v>1.2310000000000001</v>
       </c>
-      <c r="M113" s="41">
+      <c r="M115" s="41">
         <f t="shared" si="27"/>
         <v>12.31</v>
       </c>
-      <c r="O113" t="s">
+      <c r="O115" t="s">
         <v>343</v>
       </c>
     </row>
-    <row r="114" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="J114" s="40">
+    <row r="116" spans="2:15" x14ac:dyDescent="0.3">
+      <c r="J116" s="40">
         <f t="shared" si="25"/>
         <v>0</v>
       </c>
-      <c r="L114" s="41">
+      <c r="L116" s="41">
         <f t="shared" si="26"/>
         <v>0</v>
       </c>
-      <c r="M114" s="41">
+      <c r="M116" s="41">
         <f t="shared" si="27"/>
         <v>0</v>
       </c>
     </row>
-    <row r="115" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="J115" s="40">
+    <row r="117" spans="2:15" x14ac:dyDescent="0.3">
+      <c r="J117" s="40">
         <f t="shared" si="25"/>
         <v>0</v>
       </c>
-      <c r="L115" s="41">
+      <c r="L117" s="41">
         <f t="shared" si="26"/>
         <v>0</v>
       </c>
-      <c r="M115" s="41">
+      <c r="M117" s="41">
         <f t="shared" si="27"/>
         <v>0</v>
       </c>
     </row>
-    <row r="144" spans="17:33" x14ac:dyDescent="0.25">
-      <c r="Q144" s="36"/>
-      <c r="R144" s="36"/>
-      <c r="S144" s="36"/>
-      <c r="T144" s="36"/>
-      <c r="U144" s="36"/>
-      <c r="V144" s="36"/>
-      <c r="W144" s="36"/>
-      <c r="X144" s="36"/>
-      <c r="Y144" s="36"/>
-      <c r="Z144" s="36"/>
-      <c r="AA144" s="36"/>
-      <c r="AB144" s="36"/>
-      <c r="AC144" s="36"/>
-      <c r="AD144" s="36"/>
-      <c r="AE144" s="36"/>
-      <c r="AF144" s="36"/>
-      <c r="AG144" s="36"/>
-    </row>
-    <row r="145" spans="16:16" x14ac:dyDescent="0.25">
-      <c r="P145" s="36"/>
+    <row r="146" spans="16:33" x14ac:dyDescent="0.3">
+      <c r="Q146" s="36"/>
+      <c r="R146" s="36"/>
+      <c r="S146" s="36"/>
+      <c r="T146" s="36"/>
+      <c r="U146" s="36"/>
+      <c r="V146" s="36"/>
+      <c r="W146" s="36"/>
+      <c r="X146" s="36"/>
+      <c r="Y146" s="36"/>
+      <c r="Z146" s="36"/>
+      <c r="AA146" s="36"/>
+      <c r="AB146" s="36"/>
+      <c r="AC146" s="36"/>
+      <c r="AD146" s="36"/>
+      <c r="AE146" s="36"/>
+      <c r="AF146" s="36"/>
+      <c r="AG146" s="36"/>
+    </row>
+    <row r="147" spans="16:33" x14ac:dyDescent="0.3">
+      <c r="P147" s="36"/>
     </row>
   </sheetData>
   <mergeCells count="3">
@@ -6192,14 +6268,14 @@
     <mergeCell ref="A40:C40"/>
   </mergeCells>
   <hyperlinks>
-    <hyperlink ref="O74" r:id="rId1" xr:uid="{02ED6716-7816-4B3E-9192-4DE2DB3E7904}"/>
-    <hyperlink ref="O84" r:id="rId2" xr:uid="{C5139CD4-D29C-4F40-ACA0-995CCE988BEE}"/>
+    <hyperlink ref="O76" r:id="rId1" xr:uid="{02ED6716-7816-4B3E-9192-4DE2DB3E7904}"/>
+    <hyperlink ref="O86" r:id="rId2" xr:uid="{C5139CD4-D29C-4F40-ACA0-995CCE988BEE}"/>
     <hyperlink ref="O12" r:id="rId3" xr:uid="{71563680-2C44-46CE-8289-648766517570}"/>
     <hyperlink ref="O31" r:id="rId4" xr:uid="{610CCE72-9DC7-41A4-88EE-87699EEA8DFC}"/>
     <hyperlink ref="O28" r:id="rId5" xr:uid="{92CB4CE6-0C06-4100-B560-42F52BF2C637}"/>
-    <hyperlink ref="O85" r:id="rId6" xr:uid="{255C0494-26CB-426C-AA38-5D391BD7768A}"/>
+    <hyperlink ref="O87" r:id="rId6" xr:uid="{255C0494-26CB-426C-AA38-5D391BD7768A}"/>
     <hyperlink ref="O32" r:id="rId7" xr:uid="{EF086B6A-81CA-486D-AAFF-04B6DFE7F47D}"/>
-    <hyperlink ref="O79" r:id="rId8" xr:uid="{9479A087-8561-4FC8-9104-391F1A93A46C}"/>
+    <hyperlink ref="O81" r:id="rId8" xr:uid="{9479A087-8561-4FC8-9104-391F1A93A46C}"/>
     <hyperlink ref="O34" r:id="rId9" xr:uid="{FCF07C8B-3453-4B90-A45C-5C23870E3AA3}"/>
     <hyperlink ref="O11" r:id="rId10" xr:uid="{AD1729D6-FBF8-42FF-820E-275F653BB3D6}"/>
     <hyperlink ref="O38" r:id="rId11" xr:uid="{C1DB9D99-DB62-4744-A864-543646FAE8AA}"/>
@@ -6222,12 +6298,12 @@
     <hyperlink ref="O6" r:id="rId28" xr:uid="{F9E4BECB-9011-4137-823B-2ADAF0EA1EA6}"/>
     <hyperlink ref="O7" r:id="rId29" xr:uid="{50FB6E1D-77D1-4B82-AE6A-492732D8D216}"/>
     <hyperlink ref="O9" r:id="rId30" xr:uid="{1353EC35-CD14-405B-ADC0-88CEEAF33AB6}"/>
-    <hyperlink ref="O76" r:id="rId31" xr:uid="{EEFAB4B2-4940-4C60-8F53-D695D2AD9D04}"/>
-    <hyperlink ref="O78" r:id="rId32" xr:uid="{3C991A0B-A360-43EB-B2D4-4D48F29056CE}"/>
-    <hyperlink ref="O77" r:id="rId33" xr:uid="{7676F691-353A-4745-A640-8245F75CC9CC}"/>
+    <hyperlink ref="O78" r:id="rId31" xr:uid="{EEFAB4B2-4940-4C60-8F53-D695D2AD9D04}"/>
+    <hyperlink ref="O80" r:id="rId32" xr:uid="{3C991A0B-A360-43EB-B2D4-4D48F29056CE}"/>
+    <hyperlink ref="O79" r:id="rId33" xr:uid="{7676F691-353A-4745-A640-8245F75CC9CC}"/>
     <hyperlink ref="O20" r:id="rId34" xr:uid="{DFA44B43-C7A0-43CA-989D-D3BFE142F1D4}"/>
     <hyperlink ref="O15" r:id="rId35" xr:uid="{EAFCD7F5-88CD-4223-99C2-008E32FA2D0C}"/>
-    <hyperlink ref="O82" r:id="rId36" xr:uid="{923561A7-2757-49F4-9B5E-10369AFD95F4}"/>
+    <hyperlink ref="O84" r:id="rId36" xr:uid="{923561A7-2757-49F4-9B5E-10369AFD95F4}"/>
     <hyperlink ref="O22" r:id="rId37" xr:uid="{4914D6D6-5978-4D9F-A2F8-0591E99210F5}"/>
     <hyperlink ref="O21" r:id="rId38" xr:uid="{42ABB6F0-0AC8-4536-B11D-3099C7EEF74D}"/>
     <hyperlink ref="O23" r:id="rId39" xr:uid="{60F5A35C-7655-47B5-A74B-F93AF3445E69}"/>
@@ -6236,7 +6312,7 @@
     <hyperlink ref="O36" r:id="rId42" xr:uid="{650F4D0A-17AB-4D08-A591-5D6AD702A5D1}"/>
     <hyperlink ref="O39" r:id="rId43" xr:uid="{966DB76C-4FE9-409E-AB1D-21E89B358050}"/>
     <hyperlink ref="O42" r:id="rId44" display="https://www.amazon.ca/WOVTE-Reusable-Toddlers-Silicone-Cleaning/dp/B07KVTYG5X" xr:uid="{19A5D70E-254D-47BA-81C4-7B2B773555CF}"/>
-    <hyperlink ref="O100" r:id="rId45" xr:uid="{B3A0D2F8-3D95-44B9-BBD1-089933FB86C4}"/>
+    <hyperlink ref="O102" r:id="rId45" xr:uid="{B3A0D2F8-3D95-44B9-BBD1-089933FB86C4}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId46"/>
@@ -6244,12 +6320,14 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <TaxCatchAll xmlns="715913e6-4bf0-458f-8160-f18e142d04ff" xsi:nil="true"/>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="e718a8af-5d48-45b1-a7fb-cef00c107a7a">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+  </documentManagement>
+</p:properties>
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -6474,35 +6552,50 @@
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <TaxCatchAll xmlns="715913e6-4bf0-458f-8160-f18e142d04ff" xsi:nil="true"/>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="e718a8af-5d48-45b1-a7fb-cef00c107a7a">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-  </documentManagement>
-</p:properties>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{4740145F-09D2-466B-B9A2-2798696B0ADF}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{57C9FC67-5541-4CD4-9C4D-BDD1FC789ADC}"/>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E4958292-C6C4-482B-887A-6CF9FB19AB74}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
     <ds:schemaRef ds:uri="72c39c84-b0a3-45a2-a38c-ff46bb47f11f"/>
     <ds:schemaRef ds:uri="cf9f6c1f-8ad0-4eb8-bb2b-fb0b622a341e"/>
+    <ds:schemaRef ds:uri="715913e6-4bf0-458f-8160-f18e142d04ff"/>
+    <ds:schemaRef ds:uri="e718a8af-5d48-45b1-a7fb-cef00c107a7a"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{57C9FC67-5541-4CD4-9C4D-BDD1FC789ADC}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="e718a8af-5d48-45b1-a7fb-cef00c107a7a"/>
+    <ds:schemaRef ds:uri="715913e6-4bf0-458f-8160-f18e142d04ff"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{4740145F-09D2-466B-B9A2-2798696B0ADF}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>